<commit_message>
International trade er med
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCE0BACC-DB94-47F6-8430-C39828A69CB2}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876C10DE-5E4B-4789-B29F-FCE7E60141BE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{29A67EE3-41B7-4DDB-B48A-850B5DE5423E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="1" shapeId="0" xr:uid="{BCDEF17F-9BC4-494F-8612-27052E0883A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>Year</t>
   </si>
@@ -226,13 +252,25 @@
     <t>DE3</t>
   </si>
   <si>
-    <t>TB_ELCC_DE1_DE2_01</t>
-  </si>
-  <si>
-    <t>TB_ELCC_DE1_DE3_01</t>
-  </si>
-  <si>
     <t>TB_ELCC_DE2_DE3_01</t>
+  </si>
+  <si>
+    <t>DE4</t>
+  </si>
+  <si>
+    <t>DE5</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE2_DE5_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE3_DE4_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE3_DE5_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE4_DE5_01</t>
   </si>
 </sst>
 </file>
@@ -242,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +379,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +470,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -445,13 +495,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -484,13 +535,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>101601</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>169335</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
@@ -1512,10 +1563,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1526,29 +1577,31 @@
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="23.36328125" customWidth="1"/>
-    <col min="10" max="10" width="19.453125" customWidth="1"/>
-    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="23.36328125" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" customWidth="1"/>
     <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1570,77 +1623,84 @@
       <c r="H4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5">
-        <v>2010</v>
-      </c>
-      <c r="F5">
-        <v>0.97</v>
+        <v>2016</v>
       </c>
       <c r="G5">
         <v>0.97</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="H5">
+        <v>0.97</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>0.92</v>
-      </c>
       <c r="G6">
         <v>0.92</v>
       </c>
-      <c r="I6" s="10" t="str">
-        <f>I5</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0.92</v>
+      </c>
+      <c r="K6" s="10" t="str">
+        <f>K5</f>
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="F7">
-        <v>50</v>
-      </c>
       <c r="G7">
         <v>50</v>
       </c>
-      <c r="I7" s="10" t="str">
-        <f>I6</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="K7" s="10" t="str">
+        <f>K6</f>
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
       <c r="G8" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="10" t="str">
-        <f t="shared" ref="I8:I13" si="0">I7</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H8" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="10" t="str">
+        <f t="shared" ref="K8:K13" si="0">K7</f>
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
         <v>43</v>
@@ -1649,25 +1709,26 @@
         <v>10</v>
       </c>
       <c r="E9" s="10">
-        <v>2010</v>
-      </c>
-      <c r="F9" s="10">
-        <v>100</v>
+        <v>2016</v>
       </c>
       <c r="G9" s="10">
-        <v>100</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="str">
+        <v>8634</v>
+      </c>
+      <c r="H9" s="10">
+        <v>8634</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>10</v>
@@ -1675,20 +1736,21 @@
       <c r="E10" s="10">
         <v>2020</v>
       </c>
-      <c r="F10" s="10">
-        <v>150</v>
-      </c>
       <c r="G10" s="10">
-        <v>150</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="str">
+        <v>12000</v>
+      </c>
+      <c r="H10" s="10">
+        <v>12000</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
         <v>11</v>
@@ -1699,20 +1761,21 @@
       <c r="E11" s="10">
         <v>2030</v>
       </c>
-      <c r="F11" s="10">
-        <v>1000</v>
-      </c>
       <c r="G11" s="10">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="str">
+        <v>20000</v>
+      </c>
+      <c r="H11" s="10">
+        <v>20000</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
       <c r="C12" t="s">
         <v>11</v>
@@ -1723,132 +1786,133 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="9">
-        <v>5</v>
-      </c>
       <c r="G12" s="9">
         <v>5</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10" t="str">
+      <c r="H12" s="9">
+        <v>5</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21" t="s">
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="22">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="20">
+        <f>'Data New Transmission'!X15</f>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="H13" s="20">
         <f>'Data New Transmission'!W15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="G13" s="22">
-        <f>'Data New Transmission'!X15</f>
-        <v>0.26750000000000002</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20" t="str">
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="J13" s="20" t="s">
+        <v>TB_ELCC_DE2_DE3_01</v>
+      </c>
+      <c r="L13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14">
-        <v>2010</v>
-      </c>
-      <c r="F14">
+        <v>2016</v>
+      </c>
+      <c r="G14">
         <v>0.97</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>0.97</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K14" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>0.92</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>0.92</v>
       </c>
-      <c r="I15" s="10" t="str">
-        <f>I14</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K15" s="10" t="str">
+        <f>K14</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>50</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>50</v>
       </c>
-      <c r="I16" s="10" t="str">
-        <f>I15</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="10" t="str">
+        <f>K15</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8">
+      <c r="J17" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="I17" s="10" t="str">
-        <f t="shared" ref="I17:I21" si="1">I16</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="10" t="str">
+        <f t="shared" ref="K17:K21" si="1">K16</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C18" s="10" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="10">
-        <v>2020</v>
-      </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10" t="str">
-        <f>I17</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+        <v>2016</v>
+      </c>
+      <c r="G18" s="10">
+        <v>3010</v>
+      </c>
+      <c r="J18" s="10">
+        <v>3010</v>
+      </c>
+      <c r="K18" s="10" t="str">
+        <f>K17</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C19" s="10" t="s">
         <v>11</v>
       </c>
@@ -1856,214 +1920,665 @@
         <v>10</v>
       </c>
       <c r="E19" s="10">
-        <v>2035</v>
-      </c>
-      <c r="F19" s="10">
-        <v>500</v>
-      </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10">
-        <v>500</v>
-      </c>
-      <c r="I19" s="10" t="str">
+        <v>2020</v>
+      </c>
+      <c r="G19" s="10">
+        <v>12000</v>
+      </c>
+      <c r="J19" s="10">
+        <v>12000</v>
+      </c>
+      <c r="K19" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="10">
+        <v>2030</v>
+      </c>
+      <c r="G20" s="10">
+        <v>20000</v>
+      </c>
+      <c r="J20" s="10">
+        <v>20000</v>
+      </c>
+      <c r="K20" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
-      <c r="F20" s="9">
+      <c r="G21" s="9">
         <v>5</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9">
+      <c r="J21" s="9">
         <v>5</v>
       </c>
-      <c r="I20" s="10" t="str">
+      <c r="K21" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21" t="s">
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="22">
-        <f>F13*2</f>
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22">
-        <f>F21</f>
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="I21" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-      <c r="J21" s="20" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="20">
+        <f>'Data New Transmission'!X24</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="20">
+        <f>'Data New Transmission'!W24</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="18" t="str">
+        <f>K20</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+      <c r="L22" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D22" t="s">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E22">
-        <v>2010</v>
-      </c>
-      <c r="G22">
+      <c r="E23">
+        <v>2016</v>
+      </c>
+      <c r="H23">
         <v>0.97</v>
       </c>
-      <c r="H22">
+      <c r="I23">
         <v>0.97</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D23" t="s">
+      <c r="K23" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="G23">
+      <c r="H24">
         <v>0.92</v>
       </c>
-      <c r="H23">
+      <c r="I24">
         <v>0.92</v>
       </c>
-      <c r="I23" s="10" t="str">
-        <f>I22</f>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D24" t="s">
+      <c r="K24" s="10" t="str">
+        <f>K23</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="G24">
+      <c r="H25">
         <v>50</v>
       </c>
-      <c r="H24">
+      <c r="I25">
         <v>50</v>
       </c>
-      <c r="I24" s="10" t="str">
-        <f>I23</f>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D25" t="s">
+      <c r="K25" s="10" t="str">
+        <f>K24</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="8">
+      <c r="H26" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="H25" s="8">
+      <c r="I26" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="I25" s="10" t="str">
-        <f t="shared" ref="I25" si="2">I24</f>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="10">
-        <v>2020</v>
-      </c>
-      <c r="G26" s="10">
-        <v>0</v>
-      </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-      <c r="I26" s="10" t="str">
-        <f>I25</f>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J26" s="8"/>
+      <c r="K26" s="10" t="str">
+        <f t="shared" ref="K26:K30" si="2">K25</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="10" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="10">
-        <v>2035</v>
-      </c>
-      <c r="G27" s="10">
-        <v>500</v>
-      </c>
-      <c r="H27" s="10">
-        <v>500</v>
-      </c>
-      <c r="I27" s="10" t="str">
-        <f t="shared" ref="I27:I29" si="3">I26</f>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
+        <v>2016</v>
+      </c>
+      <c r="H27" s="22">
+        <f>14416</f>
+        <v>14416</v>
+      </c>
+      <c r="I27" s="22">
+        <f>14416</f>
+        <v>14416</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10" t="str">
+        <f>K26</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="10">
+        <v>2020</v>
+      </c>
+      <c r="H28" s="10">
+        <v>17000</v>
+      </c>
+      <c r="I28" s="10">
+        <v>17000</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="10">
+        <v>2030</v>
+      </c>
+      <c r="H29" s="10">
+        <v>25000</v>
+      </c>
+      <c r="I29" s="10">
+        <v>25000</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
         <v>0</v>
       </c>
-      <c r="G28" s="9">
+      <c r="H30" s="9">
         <v>5</v>
       </c>
-      <c r="H28" s="9">
+      <c r="I30" s="9">
         <v>5</v>
       </c>
-      <c r="I28" s="10" t="str">
+      <c r="J30" s="9"/>
+      <c r="K30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="20">
+        <f>'Data New Transmission'!X33</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="20">
+        <f>'Data New Transmission'!Y33</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="20"/>
+      <c r="K31" s="18" t="str">
+        <f>K29</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>2016</v>
+      </c>
+      <c r="H32">
+        <v>0.97</v>
+      </c>
+      <c r="J32">
+        <v>0.97</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>0.92</v>
+      </c>
+      <c r="J33">
+        <v>0.92</v>
+      </c>
+      <c r="K33" s="10" t="str">
+        <f>K32</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+      <c r="J34">
+        <v>50</v>
+      </c>
+      <c r="K34" s="10" t="str">
+        <f>K33</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J35" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K35" s="10" t="str">
+        <f t="shared" ref="K35:K39" si="3">K34</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H36" s="22">
+        <v>6020</v>
+      </c>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22">
+        <v>6020</v>
+      </c>
+      <c r="K36" s="10" t="str">
+        <f>K35</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C37" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="10">
+        <v>2020</v>
+      </c>
+      <c r="H37" s="10">
+        <v>17000</v>
+      </c>
+      <c r="J37" s="10">
+        <v>17000</v>
+      </c>
+      <c r="K37" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C29" s="18"/>
-      <c r="D29" s="18" t="s">
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C38" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="10">
+        <v>2030</v>
+      </c>
+      <c r="H38" s="10">
+        <v>25000</v>
+      </c>
+      <c r="J38" s="10">
+        <v>25000</v>
+      </c>
+      <c r="K38" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>5</v>
+      </c>
+      <c r="J39" s="9">
+        <v>5</v>
+      </c>
+      <c r="K39" s="10" t="str">
+        <f t="shared" si="3"/>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C40" s="19"/>
+      <c r="D40" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="G29" s="19">
-        <f>F21</f>
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="H29" s="19">
-        <f>G29</f>
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="I29" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-      <c r="J29" s="20" t="s">
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="20">
+        <f>'Data New Transmission'!X42</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="20">
+        <f>'Data New Transmission'!Y42</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="18" t="str">
+        <f>K38</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+      <c r="L40" s="18" t="s">
         <v>46</v>
       </c>
     </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>2016</v>
+      </c>
+      <c r="I41">
+        <v>0.97</v>
+      </c>
+      <c r="J41">
+        <v>0.97</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42">
+        <v>0.92</v>
+      </c>
+      <c r="J42">
+        <v>0.92</v>
+      </c>
+      <c r="K42" s="10" t="str">
+        <f>K41</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43">
+        <v>50</v>
+      </c>
+      <c r="J43">
+        <v>50</v>
+      </c>
+      <c r="K43" s="10" t="str">
+        <f>K42</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J44" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K44" s="10" t="str">
+        <f t="shared" ref="K44:K48" si="4">K43</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C45" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="10">
+        <v>2016</v>
+      </c>
+      <c r="I45" s="22">
+        <v>3010</v>
+      </c>
+      <c r="J45" s="22">
+        <v>3010</v>
+      </c>
+      <c r="K45" s="10" t="str">
+        <f>K44</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="10">
+        <v>2020</v>
+      </c>
+      <c r="I46" s="10">
+        <v>17000</v>
+      </c>
+      <c r="J46" s="10">
+        <v>17000</v>
+      </c>
+      <c r="K46" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C47" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="10">
+        <v>2030</v>
+      </c>
+      <c r="I47" s="10">
+        <v>25000</v>
+      </c>
+      <c r="J47" s="10">
+        <v>25000</v>
+      </c>
+      <c r="K47" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="I48" s="9">
+        <v>5</v>
+      </c>
+      <c r="J48" s="9">
+        <v>5</v>
+      </c>
+      <c r="K48" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="I49" s="20">
+        <f>'Data New Transmission'!X51</f>
+        <v>0</v>
+      </c>
+      <c r="J49" s="20">
+        <f>'Data New Transmission'!Y51</f>
+        <v>0</v>
+      </c>
+      <c r="K49" s="18" t="str">
+        <f>K47</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="K50" s="10"/>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="K51" s="10"/>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2078,7 +2593,7 @@
   </sheetPr>
   <dimension ref="B1:AA28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
@@ -2333,48 +2848,48 @@
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="M2" s="23" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="M2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
       <c r="AH3" s="15" t="s">
         <v>36</v>
       </c>
@@ -2580,21 +3095,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -2817,24 +3317,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2851,4 +3349,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update af trade ml. regioner
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876C10DE-5E4B-4789-B29F-FCE7E60141BE}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17659222-BD61-4108-B279-C9030E448BC3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>TB_ELCC_DE4_DE5_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE1_DE2_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE1_DE3_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE1_DE4_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DE1_DE5_01</t>
   </si>
 </sst>
 </file>
@@ -498,11 +510,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1563,10 +1575,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1809,7 +1821,7 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="20">
-        <f>'Data New Transmission'!X15</f>
+        <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
       <c r="H13" s="20">
@@ -1984,14 +1996,14 @@
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="20">
-        <f>'Data New Transmission'!X24</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
       <c r="J22" s="20">
-        <f>'Data New Transmission'!W24</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="K22" s="18" t="str">
         <f>K20</f>
@@ -2074,11 +2086,11 @@
       <c r="E27" s="10">
         <v>2016</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="21">
         <f>14416</f>
         <v>14416</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="21">
         <f>14416</f>
         <v>14416</v>
       </c>
@@ -2163,12 +2175,12 @@
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="20">
-        <f>'Data New Transmission'!X33</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="I31" s="20">
-        <f>'Data New Transmission'!Y33</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="J31" s="20"/>
       <c r="K31" s="18" t="str">
@@ -2251,11 +2263,11 @@
       <c r="E36" s="10">
         <v>2016</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="21">
         <v>6020</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22">
+      <c r="I36" s="21"/>
+      <c r="J36" s="21">
         <v>6020</v>
       </c>
       <c r="K36" s="10" t="str">
@@ -2335,13 +2347,13 @@
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
       <c r="H40" s="20">
-        <f>'Data New Transmission'!X42</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="20">
-        <f>'Data New Transmission'!Y42</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="K40" s="18" t="str">
         <f>K38</f>
@@ -2423,10 +2435,10 @@
       <c r="E45" s="10">
         <v>2016</v>
       </c>
-      <c r="I45" s="22">
+      <c r="I45" s="21">
         <v>3010</v>
       </c>
-      <c r="J45" s="22">
+      <c r="J45" s="21">
         <v>3010</v>
       </c>
       <c r="K45" s="10" t="str">
@@ -2506,12 +2518,12 @@
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
       <c r="I49" s="20">
-        <f>'Data New Transmission'!X51</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="J49" s="20">
-        <f>'Data New Transmission'!Y51</f>
-        <v>0</v>
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
       </c>
       <c r="K49" s="18" t="str">
         <f>K47</f>
@@ -2522,60 +2534,528 @@
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="K50" s="10"/>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>2016</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="K51" s="10"/>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="K51" s="10" t="str">
+        <f>K50</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="K52" s="10"/>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+      <c r="K52" s="10" t="str">
+        <f>K51</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="H53" s="8"/>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="G53" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I53" s="8"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="10"/>
+      <c r="K53" s="10" t="str">
+        <f t="shared" ref="K53:K56" si="5">K52</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="10"/>
+      <c r="C54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F54" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="G54" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L54" s="10"/>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="9">
+        <v>5</v>
+      </c>
+      <c r="G55" s="9">
+        <v>5</v>
+      </c>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="10" t="str">
+        <f>K50</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L55" s="10"/>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="18"/>
+      <c r="F56" s="20">
+        <v>0</v>
+      </c>
+      <c r="G56" s="20">
+        <v>0</v>
+      </c>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L56" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="57" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="H57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="10"/>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57">
+        <v>2016</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18"/>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="K58" s="10" t="str">
+        <f>K57</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59">
+        <v>100</v>
+      </c>
+      <c r="H59">
+        <v>100</v>
+      </c>
+      <c r="K59" s="10" t="str">
+        <f>K58</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="H60" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="10" t="str">
+        <f t="shared" ref="K60:K63" si="6">K59</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C61" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F61" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="H61" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L61" s="10"/>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" s="9">
+        <v>5</v>
+      </c>
+      <c r="H62" s="9">
+        <v>5</v>
+      </c>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="10" t="str">
+        <f>K57</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L62" s="10"/>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C63" s="19"/>
+      <c r="D63" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="18"/>
+      <c r="F63" s="20">
+        <v>0</v>
+      </c>
+      <c r="H63" s="20">
+        <v>0</v>
+      </c>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L63" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64">
+        <v>2016</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="K65" s="10" t="str">
+        <f>K64</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
+      <c r="I66">
+        <v>100</v>
+      </c>
+      <c r="K66" s="10" t="str">
+        <f>K65</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I67" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J67" s="8"/>
+      <c r="K67" s="10" t="str">
+        <f t="shared" ref="K67:K70" si="7">K66</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+    </row>
+    <row r="68" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C68" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F68" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I68" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L68" s="10"/>
+    </row>
+    <row r="69" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" s="9">
+        <v>5</v>
+      </c>
+      <c r="I69" s="9">
+        <v>5</v>
+      </c>
+      <c r="J69" s="9"/>
+      <c r="K69" s="10" t="str">
+        <f>K64</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L69" s="10"/>
+    </row>
+    <row r="70" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70" s="18"/>
+      <c r="F70" s="20">
+        <v>0</v>
+      </c>
+      <c r="I70" s="20">
+        <v>0</v>
+      </c>
+      <c r="J70" s="20"/>
+      <c r="K70" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L70" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71">
+        <v>2016</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72" s="10" t="str">
+        <f>K71</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73">
+        <v>100</v>
+      </c>
+      <c r="J73">
+        <v>100</v>
+      </c>
+      <c r="K73" s="10" t="str">
+        <f>K72</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J74" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K74" s="10" t="str">
+        <f t="shared" ref="K74:K77" si="8">K73</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C75" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F75" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="J75" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="K75" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+      <c r="L75" s="10"/>
+    </row>
+    <row r="76" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" s="9">
+        <v>5</v>
+      </c>
+      <c r="J76" s="9">
+        <v>5</v>
+      </c>
+      <c r="K76" s="10" t="str">
+        <f>K71</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+      <c r="L76" s="10"/>
+    </row>
+    <row r="77" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C77" s="19"/>
+      <c r="D77" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E77" s="18"/>
+      <c r="F77" s="20">
+        <v>0</v>
+      </c>
+      <c r="J77" s="20">
+        <v>0</v>
+      </c>
+      <c r="K77" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>TB_ELCC_DE1_DE5_01</v>
+      </c>
+      <c r="L77" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
@@ -2848,48 +3328,48 @@
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="M2" s="21" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="M2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
       <c r="AH3" s="15" t="s">
         <v>36</v>
       </c>
@@ -3095,6 +3575,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3317,22 +3812,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3349,21 +3846,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Nye pop og GDP
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17659222-BD61-4108-B279-C9030E448BC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DD953-B2F2-4FC2-9B57-7650742797B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="61">
   <si>
     <t>Year</t>
   </si>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>Cost allocation</t>
-  </si>
-  <si>
-    <t>FX</t>
   </si>
   <si>
     <t>Additional MW</t>
@@ -1577,8 +1574,8 @@
   </sheetPr>
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1627,19 +1624,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="I4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>1</v>
@@ -1662,7 +1659,7 @@
         <v>0.97</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1715,7 +1712,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>10</v>
@@ -1835,10 +1832,10 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
       <c r="L13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" t="s">
         <v>46</v>
-      </c>
-      <c r="N13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1855,7 +1852,7 @@
         <v>0.97</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1905,7 +1902,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C18" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>10</v>
@@ -2010,7 +2007,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
@@ -2027,7 +2024,7 @@
         <v>0.97</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
@@ -2078,7 +2075,7 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>10</v>
@@ -2188,7 +2185,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
@@ -2205,7 +2202,7 @@
         <v>0.97</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.35">
@@ -2255,7 +2252,7 @@
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C36" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>10</v>
@@ -2360,7 +2357,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
       <c r="L40" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.35">
@@ -2377,7 +2374,7 @@
         <v>0.97</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.35">
@@ -2427,7 +2424,7 @@
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C45" s="10" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>10</v>
@@ -2530,7 +2527,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.35">
@@ -2547,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.35">
@@ -2664,7 +2661,7 @@
         <v>TB_ELCC_DE1_DE2_01</v>
       </c>
       <c r="L56" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="3:12" x14ac:dyDescent="0.35">
@@ -2681,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.35">
@@ -2798,7 +2795,7 @@
         <v>TB_ELCC_DE1_DE3_01</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.35">
@@ -2815,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.35">
@@ -2928,7 +2925,7 @@
         <v>TB_ELCC_DE1_DE4_01</v>
       </c>
       <c r="L70" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.35">
@@ -2945,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="3:12" x14ac:dyDescent="0.35">
@@ -3054,7 +3051,7 @@
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
       <c r="L77" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3092,7 @@
         <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.35">
@@ -3111,7 +3108,7 @@
         <v>18</v>
       </c>
       <c r="Y4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z4" t="s">
         <v>19</v>
@@ -3575,21 +3572,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3812,24 +3794,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3846,4 +3826,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Opdateret efter snak med Mikkel
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F37BC3F4-465D-433B-988F-CFB8A857A771}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DBB6B18-60B1-47A7-B472-185C992FF638}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>TB_ELCC_DE1_DE5_01</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -1572,10 +1575,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:N77"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1705,14 +1708,14 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="10" t="str">
-        <f t="shared" ref="K8:K13" si="0">K7</f>
+        <f t="shared" ref="K8:K9" si="0">K7</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>10</v>
@@ -1735,135 +1738,111 @@
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="10">
-        <v>2020</v>
-      </c>
-      <c r="G10" s="10">
-        <v>12000</v>
-      </c>
-      <c r="H10" s="10">
-        <v>12000</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="10">
-        <v>2030</v>
-      </c>
-      <c r="G11" s="10">
-        <v>20000</v>
-      </c>
-      <c r="H11" s="10">
-        <v>20000</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="10"/>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>5</v>
-      </c>
-      <c r="H12" s="9">
-        <v>5</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>TB_ELCC_DE2_DE3_01</v>
-      </c>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="20">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="20">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H10" s="20">
         <f>'Data New Transmission'!W15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="18" t="str">
+        <f>K9</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L10" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N10" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>2016</v>
+      </c>
+      <c r="G11">
+        <v>0.97</v>
+      </c>
+      <c r="J11">
+        <v>0.97</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>0.92</v>
+      </c>
+      <c r="J12">
+        <v>0.92</v>
+      </c>
+      <c r="K12" s="10" t="str">
+        <f>K11</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="J13">
+        <v>50</v>
+      </c>
+      <c r="K13" s="10" t="str">
+        <f>K12</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="G14" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J14" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K14" s="10" t="str">
+        <f t="shared" ref="K14" si="1">K13</f>
+        <v>TB_ELCC_DE2_DE5_01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="10">
         <v>2016</v>
       </c>
-      <c r="G14">
-        <v>0.97</v>
-      </c>
-      <c r="J14">
-        <v>0.97</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15">
-        <v>0.92</v>
-      </c>
-      <c r="J15">
-        <v>0.92</v>
+      <c r="G15" s="10">
+        <v>3010</v>
+      </c>
+      <c r="J15" s="10">
+        <v>3010</v>
       </c>
       <c r="K15" s="10" t="str">
         <f>K14</f>
@@ -1871,146 +1850,144 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16">
-        <v>50</v>
-      </c>
-      <c r="J16">
-        <v>50</v>
-      </c>
-      <c r="K16" s="10" t="str">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="20">
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="20">
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="K16" s="18" t="str">
         <f>K15</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="L16" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="J17" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="K17" s="10" t="str">
-        <f t="shared" ref="K17:K21" si="1">K16</f>
-        <v>TB_ELCC_DE2_DE5_01</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="10">
+        <v>7</v>
+      </c>
+      <c r="E17">
         <v>2016</v>
       </c>
-      <c r="G18" s="10">
-        <v>3010</v>
-      </c>
-      <c r="J18" s="10">
-        <v>3010</v>
+      <c r="H17">
+        <v>0.97</v>
+      </c>
+      <c r="I17">
+        <v>0.97</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>0.92</v>
+      </c>
+      <c r="I18">
+        <v>0.92</v>
       </c>
       <c r="K18" s="10" t="str">
         <f>K17</f>
-        <v>TB_ELCC_DE2_DE5_01</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="10" t="s">
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="K19" s="10" t="str">
+        <f>K18</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I20" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="10" t="str">
+        <f t="shared" ref="K20" si="2">K19</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="10">
-        <v>2020</v>
-      </c>
-      <c r="G19" s="10">
-        <v>12000</v>
-      </c>
-      <c r="J19" s="10">
-        <v>12000</v>
-      </c>
-      <c r="K19" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>TB_ELCC_DE2_DE5_01</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="10">
-        <v>2030</v>
-      </c>
-      <c r="G20" s="10">
-        <v>20000</v>
-      </c>
-      <c r="J20" s="10">
-        <v>20000</v>
-      </c>
-      <c r="K20" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>TB_ELCC_DE2_DE5_01</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9">
-        <v>5</v>
-      </c>
-      <c r="J21" s="9">
-        <v>5</v>
-      </c>
+      <c r="E21" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H21" s="21">
+        <f>14416</f>
+        <v>14416</v>
+      </c>
+      <c r="I21" s="21">
+        <f>14416</f>
+        <v>14416</v>
+      </c>
+      <c r="J21" s="10"/>
       <c r="K21" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>TB_ELCC_DE2_DE5_01</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="18"/>
+        <f>K20</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
-      <c r="G22" s="20">
+      <c r="G22" s="18"/>
+      <c r="H22" s="20">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="20">
+      <c r="I22" s="20">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
+      <c r="J22" s="20"/>
       <c r="K22" s="18" t="str">
-        <f>K20</f>
-        <v>TB_ELCC_DE2_DE5_01</v>
+        <f>K21</f>
+        <v>TB_ELCC_DE3_DE4_01</v>
       </c>
       <c r="L22" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -2020,62 +1997,61 @@
       <c r="H23">
         <v>0.97</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.97</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="H24">
         <v>0.92</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.92</v>
       </c>
       <c r="K24" s="10" t="str">
         <f>K23</f>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="H25">
         <v>50</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>50</v>
       </c>
       <c r="K25" s="10" t="str">
         <f>K24</f>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="I26" s="8">
+      <c r="J26" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J26" s="8"/>
       <c r="K26" s="10" t="str">
-        <f t="shared" ref="K26:K30" si="2">K25</f>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+        <f t="shared" ref="K26" si="3">K25</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="10" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>10</v>
@@ -2084,363 +2060,345 @@
         <v>2016</v>
       </c>
       <c r="H27" s="21">
-        <f>14416</f>
-        <v>14416</v>
-      </c>
-      <c r="I27" s="21">
-        <f>14416</f>
-        <v>14416</v>
-      </c>
-      <c r="J27" s="10"/>
+        <v>6020</v>
+      </c>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21">
+        <v>6020</v>
+      </c>
       <c r="K27" s="10" t="str">
         <f>K26</f>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C28" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="10">
-        <v>2020</v>
-      </c>
-      <c r="H28" s="10">
-        <v>17000</v>
-      </c>
-      <c r="I28" s="10">
-        <v>17000</v>
-      </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C29" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="10">
-        <v>2030</v>
-      </c>
-      <c r="H29" s="10">
-        <v>25000</v>
-      </c>
-      <c r="I29" s="10">
-        <v>25000</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9">
-        <v>5</v>
-      </c>
-      <c r="I30" s="9">
-        <v>5</v>
-      </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="s">
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="20">
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="20">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="I31" s="20">
+      <c r="I28" s="18"/>
+      <c r="J28" s="20">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="18" t="str">
+      <c r="K28" s="18" t="str">
+        <f>K27</f>
+        <v>TB_ELCC_DE3_DE5_01</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>2016</v>
+      </c>
+      <c r="I29">
+        <v>0.97</v>
+      </c>
+      <c r="J29">
+        <v>0.97</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30">
+        <v>0.92</v>
+      </c>
+      <c r="J30">
+        <v>0.92</v>
+      </c>
+      <c r="K30" s="10" t="str">
         <f>K29</f>
-        <v>TB_ELCC_DE3_DE4_01</v>
-      </c>
-      <c r="L31" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31">
+        <v>50</v>
+      </c>
+      <c r="J31">
+        <v>50</v>
+      </c>
+      <c r="K31" s="10" t="str">
+        <f>K30</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="I32" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J32" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K32" s="10" t="str">
+        <f t="shared" ref="K32" si="4">K31</f>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C33" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="10">
         <v>2016</v>
       </c>
-      <c r="H32">
-        <v>0.97</v>
-      </c>
-      <c r="J32">
-        <v>0.97</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33">
-        <v>0.92</v>
-      </c>
-      <c r="J33">
-        <v>0.92</v>
+      <c r="I33" s="21">
+        <v>3010</v>
+      </c>
+      <c r="J33" s="21">
+        <v>3010</v>
       </c>
       <c r="K33" s="10" t="str">
         <f>K32</f>
-        <v>TB_ELCC_DE3_DE5_01</v>
+        <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34">
-        <v>50</v>
-      </c>
-      <c r="J34">
-        <v>50</v>
-      </c>
-      <c r="K34" s="10" t="str">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="I34" s="20">
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="J34" s="20">
+        <f>'Data New Transmission'!$X$15</f>
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="K34" s="18" t="str">
         <f>K33</f>
-        <v>TB_ELCC_DE3_DE5_01</v>
+        <v>TB_ELCC_DE4_DE5_01</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="J35" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="K35" s="10" t="str">
-        <f t="shared" ref="K35:K39" si="3">K34</f>
-        <v>TB_ELCC_DE3_DE5_01</v>
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <v>2016</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C36" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="10">
-        <v>2016</v>
-      </c>
-      <c r="H36" s="21">
-        <v>6020</v>
-      </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21">
-        <v>6020</v>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
       </c>
       <c r="K36" s="10" t="str">
         <f>K35</f>
-        <v>TB_ELCC_DE3_DE5_01</v>
+        <v>TB_ELCC_DE1_DE2_01</v>
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C37" s="10" t="s">
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>100</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+      <c r="K37" s="10" t="str">
+        <f>K36</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="G38" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="10" t="str">
+        <f t="shared" ref="K38:K41" si="5">K37</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="10">
-        <v>2020</v>
-      </c>
-      <c r="H37" s="10">
-        <v>17000</v>
-      </c>
-      <c r="J37" s="10">
-        <v>17000</v>
-      </c>
-      <c r="K37" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_ELCC_DE3_DE5_01</v>
-      </c>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C38" s="10" t="s">
+      <c r="E39" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F39" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="G39" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L39" s="10"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D40" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="10">
-        <v>2030</v>
-      </c>
-      <c r="H38" s="10">
-        <v>25000</v>
-      </c>
-      <c r="J38" s="10">
-        <v>25000</v>
-      </c>
-      <c r="K38" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_ELCC_DE3_DE5_01</v>
-      </c>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39">
+      <c r="E40">
         <v>0</v>
       </c>
-      <c r="H39" s="9">
+      <c r="F40" s="9">
         <v>5</v>
       </c>
-      <c r="J39" s="9">
+      <c r="G40" s="9">
         <v>5</v>
       </c>
-      <c r="K39" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>TB_ELCC_DE3_DE5_01</v>
-      </c>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C40" s="19"/>
-      <c r="D40" s="19" t="s">
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="10" t="str">
+        <f>K35</f>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L40" s="10"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="20">
-        <f>'Data New Transmission'!$X$15</f>
-        <v>0.26750000000000002</v>
-      </c>
-      <c r="I40" s="18"/>
-      <c r="J40" s="20">
-        <f>'Data New Transmission'!$X$15</f>
-        <v>0.26750000000000002</v>
-      </c>
-      <c r="K40" s="18" t="str">
-        <f>K38</f>
-        <v>TB_ELCC_DE3_DE5_01</v>
-      </c>
-      <c r="L40" s="18" t="s">
+      <c r="E41" s="18"/>
+      <c r="F41" s="20">
+        <v>0</v>
+      </c>
+      <c r="G41" s="20">
+        <v>0</v>
+      </c>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="18" t="str">
+        <f t="shared" si="5"/>
+        <v>TB_ELCC_DE1_DE2_01</v>
+      </c>
+      <c r="L41" s="18" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41">
-        <v>2016</v>
-      </c>
-      <c r="I41">
-        <v>0.97</v>
-      </c>
-      <c r="J41">
-        <v>0.97</v>
-      </c>
-      <c r="K41" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I42">
-        <v>0.92</v>
-      </c>
-      <c r="J42">
-        <v>0.92</v>
-      </c>
-      <c r="K42" s="10" t="str">
-        <f>K41</f>
-        <v>TB_ELCC_DE4_DE5_01</v>
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>2016</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43">
-        <v>50</v>
-      </c>
-      <c r="J43">
-        <v>50</v>
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
       </c>
       <c r="K43" s="10" t="str">
         <f>K42</f>
-        <v>TB_ELCC_DE4_DE5_01</v>
+        <v>TB_ELCC_DE1_DE3_01</v>
       </c>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>100</v>
+      </c>
+      <c r="K44" s="10" t="str">
+        <f>K43</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
         <v>8</v>
       </c>
-      <c r="I44" s="8">
+      <c r="F45" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J44" s="8">
+      <c r="H45" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K44" s="10" t="str">
-        <f t="shared" ref="K44:K48" si="4">K43</f>
-        <v>TB_ELCC_DE4_DE5_01</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C45" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="10">
-        <v>2016</v>
-      </c>
-      <c r="I45" s="21">
-        <v>3010</v>
-      </c>
-      <c r="J45" s="21">
-        <v>3010</v>
-      </c>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="10" t="str">
-        <f>K44</f>
-        <v>TB_ELCC_DE4_DE5_01</v>
+        <f t="shared" ref="K45:K48" si="6">K44</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.35">
@@ -2451,606 +2409,321 @@
         <v>10</v>
       </c>
       <c r="E46" s="10">
-        <v>2020</v>
-      </c>
-      <c r="I46" s="10">
-        <v>17000</v>
-      </c>
-      <c r="J46" s="10">
-        <v>17000</v>
-      </c>
+        <v>2016</v>
+      </c>
+      <c r="F46" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="H46" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
       <c r="K46" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>TB_ELCC_DE4_DE5_01</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L46" s="10"/>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C47" s="10" t="s">
+      <c r="C47" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="10">
-        <v>2030</v>
-      </c>
-      <c r="I47" s="10">
-        <v>25000</v>
-      </c>
-      <c r="J47" s="10">
-        <v>25000</v>
-      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="9">
+        <v>5</v>
+      </c>
+      <c r="H47" s="9">
+        <v>5</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
       <c r="K47" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>TB_ELCC_DE4_DE5_01</v>
-      </c>
+        <f>K42</f>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L47" s="10"/>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48">
+      <c r="C48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="18"/>
+      <c r="F48" s="20">
         <v>0</v>
       </c>
-      <c r="I48" s="9">
-        <v>5</v>
-      </c>
-      <c r="J48" s="9">
-        <v>5</v>
-      </c>
-      <c r="K48" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>TB_ELCC_DE4_DE5_01</v>
+      <c r="H48" s="20">
+        <v>0</v>
+      </c>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>TB_ELCC_DE1_DE3_01</v>
+      </c>
+      <c r="L48" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C49" s="19"/>
-      <c r="D49" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="I49" s="20">
-        <f>'Data New Transmission'!$X$15</f>
-        <v>0.26750000000000002</v>
-      </c>
-      <c r="J49" s="20">
-        <f>'Data New Transmission'!$X$15</f>
-        <v>0.26750000000000002</v>
-      </c>
-      <c r="K49" s="18" t="str">
-        <f>K47</f>
-        <v>TB_ELCC_DE4_DE5_01</v>
-      </c>
-      <c r="L49" s="18" t="s">
-        <v>45</v>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>2016</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50">
-        <v>2016</v>
+        <v>9</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="G50">
+      <c r="I50">
         <v>1</v>
       </c>
-      <c r="K50" s="10" t="s">
-        <v>57</v>
+      <c r="K50" s="10" t="str">
+        <f>K49</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D51" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
       </c>
       <c r="K51" s="10" t="str">
         <f>K50</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
+        <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D52" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52">
-        <v>100</v>
-      </c>
-      <c r="G52">
-        <v>100</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F52" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I52" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J52" s="8"/>
       <c r="K52" s="10" t="str">
-        <f>K51</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
+        <f t="shared" ref="K52:K55" si="7">K51</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="G53" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
+      <c r="C53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F53" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="I53" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="J53" s="10"/>
       <c r="K53" s="10" t="str">
-        <f t="shared" ref="K53:K56" si="5">K52</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L53" s="10"/>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C54" s="10" t="s">
+      <c r="C54" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="9">
+        <v>5</v>
+      </c>
+      <c r="I54" s="9">
+        <v>5</v>
+      </c>
+      <c r="J54" s="9"/>
+      <c r="K54" s="10" t="str">
+        <f>K49</f>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L54" s="10"/>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="18"/>
+      <c r="F55" s="20">
+        <v>0</v>
+      </c>
+      <c r="I55" s="20">
+        <v>0</v>
+      </c>
+      <c r="J55" s="20"/>
+      <c r="K55" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>TB_ELCC_DE1_DE4_01</v>
+      </c>
+      <c r="L55" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56">
         <v>2016</v>
       </c>
-      <c r="F54" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="G54" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="L54" s="10"/>
-    </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55" s="9">
-        <v>5</v>
-      </c>
-      <c r="G55" s="9">
-        <v>5</v>
-      </c>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="10" t="str">
-        <f>K50</f>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="L55" s="10"/>
-    </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="20">
-        <v>0</v>
-      </c>
-      <c r="G56" s="20">
-        <v>0</v>
-      </c>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>TB_ELCC_DE1_DE2_01</v>
-      </c>
-      <c r="L56" s="18" t="s">
-        <v>45</v>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D57" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57">
-        <v>2016</v>
+        <v>9</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
-      <c r="H57">
+      <c r="J57">
         <v>1</v>
       </c>
-      <c r="K57" s="10" t="s">
-        <v>58</v>
+      <c r="K57" s="10" t="str">
+        <f>K56</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="J58">
+        <v>100</v>
       </c>
       <c r="K58" s="10" t="str">
         <f>K57</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
+        <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
     <row r="59" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59">
-        <v>100</v>
-      </c>
-      <c r="H59">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="F59" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J59" s="8">
+        <v>3.1536000000000002E-2</v>
       </c>
       <c r="K59" s="10" t="str">
-        <f>K58</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
+        <f t="shared" ref="K59:K62" si="8">K58</f>
+        <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F60" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="H60" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
+      <c r="C60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="10">
+        <v>2016</v>
+      </c>
+      <c r="F60" s="10">
+        <v>10000000</v>
+      </c>
+      <c r="J60" s="10">
+        <v>10000000</v>
+      </c>
       <c r="K60" s="10" t="str">
-        <f t="shared" ref="K60:K63" si="6">K59</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C61" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="10">
-        <v>2016</v>
-      </c>
-      <c r="F61" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="H61" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-      <c r="L61" s="10"/>
-    </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C62" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62" s="9">
-        <v>5</v>
-      </c>
-      <c r="H62" s="9">
-        <v>5</v>
-      </c>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="10" t="str">
-        <f>K57</f>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-      <c r="L62" s="10"/>
-    </row>
-    <row r="63" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C63" s="19"/>
-      <c r="D63" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E63" s="18"/>
-      <c r="F63" s="20">
-        <v>0</v>
-      </c>
-      <c r="H63" s="20">
-        <v>0</v>
-      </c>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>TB_ELCC_DE1_DE3_01</v>
-      </c>
-      <c r="L63" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64">
-        <v>2016</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="K64" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-      <c r="K65" s="10" t="str">
-        <f>K64</f>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66">
-        <v>100</v>
-      </c>
-      <c r="I66">
-        <v>100</v>
-      </c>
-      <c r="K66" s="10" t="str">
-        <f>K65</f>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D67" t="s">
-        <v>8</v>
-      </c>
-      <c r="F67" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="I67" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="J67" s="8"/>
-      <c r="K67" s="10" t="str">
-        <f t="shared" ref="K67:K70" si="7">K66</f>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="68" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C68" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="10">
-        <v>2016</v>
-      </c>
-      <c r="F68" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I68" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="J68" s="10"/>
-      <c r="K68" s="10" t="str">
-        <f t="shared" si="7"/>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-      <c r="L68" s="10"/>
-    </row>
-    <row r="69" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C69" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69" s="9">
-        <v>5</v>
-      </c>
-      <c r="I69" s="9">
-        <v>5</v>
-      </c>
-      <c r="J69" s="9"/>
-      <c r="K69" s="10" t="str">
-        <f>K64</f>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-      <c r="L69" s="10"/>
-    </row>
-    <row r="70" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C70" s="19"/>
-      <c r="D70" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E70" s="18"/>
-      <c r="F70" s="20">
-        <v>0</v>
-      </c>
-      <c r="I70" s="20">
-        <v>0</v>
-      </c>
-      <c r="J70" s="20"/>
-      <c r="K70" s="18" t="str">
-        <f t="shared" si="7"/>
-        <v>TB_ELCC_DE1_DE4_01</v>
-      </c>
-      <c r="L70" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D71" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71">
-        <v>2016</v>
-      </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="K71" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-      <c r="K72" s="10" t="str">
-        <f>K71</f>
-        <v>TB_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D73" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73">
-        <v>100</v>
-      </c>
-      <c r="J73">
-        <v>100</v>
-      </c>
-      <c r="K73" s="10" t="str">
-        <f>K72</f>
-        <v>TB_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="74" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D74" t="s">
-        <v>8</v>
-      </c>
-      <c r="F74" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="J74" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="K74" s="10" t="str">
-        <f t="shared" ref="K74:K77" si="8">K73</f>
-        <v>TB_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="75" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C75" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="10">
-        <v>2016</v>
-      </c>
-      <c r="F75" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="J75" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="K75" s="10" t="str">
         <f t="shared" si="8"/>
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
-      <c r="L75" s="10"/>
-    </row>
-    <row r="76" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C76" t="s">
+      <c r="L60" s="10"/>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C61" t="s">
         <v>11</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D61" t="s">
         <v>10</v>
       </c>
-      <c r="E76">
+      <c r="E61">
         <v>0</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F61" s="9">
         <v>5</v>
       </c>
-      <c r="J76" s="9">
+      <c r="J61" s="9">
         <v>5</v>
       </c>
-      <c r="K76" s="10" t="str">
-        <f>K71</f>
+      <c r="K61" s="10" t="str">
+        <f>K56</f>
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
-      <c r="L76" s="10"/>
-    </row>
-    <row r="77" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C77" s="19"/>
-      <c r="D77" s="19" t="s">
+      <c r="L61" s="10"/>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C62" s="19"/>
+      <c r="D62" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="20">
+      <c r="E62" s="18"/>
+      <c r="F62" s="20">
         <v>0</v>
       </c>
-      <c r="J77" s="20">
+      <c r="J62" s="20">
         <v>0</v>
       </c>
-      <c r="K77" s="18" t="str">
+      <c r="K62" s="18" t="str">
         <f t="shared" si="8"/>
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
-      <c r="L77" s="18" t="s">
+      <c r="L62" s="18" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tilføjet tysk data til SUP
, IMP-MIN-EXP updateret, Forsøgt at gøre så der kan komme fuels til DE2345 powerplants
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamV/Desktop/Bachelor/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{D632E7BF-4191-D540-9A08-6D04A5FA91FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DBB6B18-60B1-47A7-B472-185C992FF638}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1704DFB-5FE2-4544-97D7-5554021B1BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23200" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId1"/>
@@ -292,7 +292,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1577,33 +1577,33 @@
   </sheetPr>
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.6328125" customWidth="1"/>
-    <col min="11" max="11" width="23.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19.453125" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1613,7 +1613,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="16" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14">
       <c r="D7" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
         <v>61</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14">
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
@@ -1766,7 +1766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14">
       <c r="D11" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14">
       <c r="C15" s="10" t="s">
         <v>61</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14">
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
@@ -1875,7 +1875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:12">
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12">
       <c r="D18" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12">
       <c r="D19" t="s">
         <v>12</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12">
       <c r="D20" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:12">
       <c r="C21" s="10" t="s">
         <v>61</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:12">
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
         <v>41</v>
@@ -1987,7 +1987,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12">
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12">
       <c r="D24" t="s">
         <v>9</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:12">
       <c r="D26" t="s">
         <v>8</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:12">
       <c r="C27" s="10" t="s">
         <v>61</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:12">
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
         <v>41</v>
@@ -2096,7 +2096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:12">
       <c r="D29" t="s">
         <v>7</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:12">
       <c r="D30" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:12">
       <c r="D31" t="s">
         <v>12</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:12">
       <c r="D32" t="s">
         <v>8</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:12">
       <c r="C33" s="10" t="s">
         <v>61</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:12">
       <c r="C34" s="19"/>
       <c r="D34" s="19" t="s">
         <v>41</v>
@@ -2203,7 +2203,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:12">
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:12">
       <c r="D36" t="s">
         <v>9</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>TB_ELCC_DE1_DE2_01</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:12">
       <c r="D37" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>TB_ELCC_DE1_DE2_01</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:12">
       <c r="D38" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>TB_ELCC_DE1_DE2_01</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:12">
       <c r="C39" s="10" t="s">
         <v>11</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="L39" s="10"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:12">
       <c r="C40" t="s">
         <v>11</v>
       </c>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="L40" s="10"/>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:12">
       <c r="C41" s="19"/>
       <c r="D41" s="19" t="s">
         <v>41</v>
@@ -2337,7 +2337,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:12">
       <c r="D42" t="s">
         <v>7</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:12">
       <c r="D43" t="s">
         <v>9</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>TB_ELCC_DE1_DE3_01</v>
       </c>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:12">
       <c r="D44" t="s">
         <v>12</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>TB_ELCC_DE1_DE3_01</v>
       </c>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:12">
       <c r="D45" t="s">
         <v>8</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>TB_ELCC_DE1_DE3_01</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:12">
       <c r="C46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2425,7 +2425,7 @@
       </c>
       <c r="L46" s="10"/>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:12">
       <c r="C47" t="s">
         <v>11</v>
       </c>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:12">
       <c r="C48" s="19"/>
       <c r="D48" s="19" t="s">
         <v>41</v>
@@ -2471,7 +2471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:12">
       <c r="D49" t="s">
         <v>7</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:12">
       <c r="D50" t="s">
         <v>9</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:12">
       <c r="D51" t="s">
         <v>12</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:12">
       <c r="D52" t="s">
         <v>8</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>TB_ELCC_DE1_DE4_01</v>
       </c>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:12">
       <c r="C53" s="10" t="s">
         <v>11</v>
       </c>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="L53" s="10"/>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:12">
       <c r="C54" t="s">
         <v>11</v>
       </c>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="L54" s="10"/>
     </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:12">
       <c r="C55" s="19"/>
       <c r="D55" s="19" t="s">
         <v>41</v>
@@ -2601,7 +2601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:12">
       <c r="D56" t="s">
         <v>7</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:12">
       <c r="D57" t="s">
         <v>9</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:12">
       <c r="D58" t="s">
         <v>12</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:12">
       <c r="D59" t="s">
         <v>8</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>TB_ELCC_DE1_DE5_01</v>
       </c>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:12">
       <c r="C60" s="10" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="L60" s="10"/>
     </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:12">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="L61" s="10"/>
     </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:12">
       <c r="C62" s="19"/>
       <c r="D62" s="19" t="s">
         <v>41</v>
@@ -2747,20 +2747,20 @@
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="24" max="24" width="10.6328125" customWidth="1"/>
-    <col min="25" max="25" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.453125" customWidth="1"/>
-    <col min="27" max="27" width="16.453125" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5" customWidth="1"/>
+    <col min="27" max="27" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:27" ht="20">
       <c r="B1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:27">
       <c r="X2" t="s">
         <v>23</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:27">
       <c r="X3" t="s">
         <v>14</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:27">
       <c r="X4" t="s">
         <v>18</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:27">
       <c r="V5" t="s">
         <v>15</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:27">
       <c r="V6" t="s">
         <v>20</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:27">
       <c r="V7" t="s">
         <v>20</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:27">
       <c r="V9" t="s">
         <v>38</v>
       </c>
@@ -2841,12 +2841,12 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:27">
       <c r="W12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:27">
       <c r="W13" t="s">
         <v>29</v>
       </c>
@@ -2854,12 +2854,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:27">
       <c r="W14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:27">
       <c r="V15" s="12"/>
       <c r="W15" s="12">
         <f>Z9/2</f>
@@ -2873,7 +2873,7 @@
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:27">
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
@@ -2881,7 +2881,7 @@
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
     </row>
-    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="22:27">
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
@@ -2889,7 +2889,7 @@
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
     </row>
-    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="22:27">
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
@@ -2897,7 +2897,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
     </row>
-    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="22:27">
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
@@ -2905,7 +2905,7 @@
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
     </row>
-    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="22:27">
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
@@ -2913,7 +2913,7 @@
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
     </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="22:27">
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
@@ -2921,7 +2921,7 @@
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
     </row>
-    <row r="22" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="22:27">
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
@@ -2929,7 +2929,7 @@
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
     </row>
-    <row r="23" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="22:27">
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
@@ -2937,7 +2937,7 @@
       <c r="Z23" s="12"/>
       <c r="AA23" s="12"/>
     </row>
-    <row r="24" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="22:27">
       <c r="V24" s="12"/>
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
@@ -2945,7 +2945,7 @@
       <c r="Z24" s="12"/>
       <c r="AA24" s="12"/>
     </row>
-    <row r="25" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="22:27">
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
@@ -2953,7 +2953,7 @@
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
     </row>
-    <row r="26" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="22:27">
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
@@ -2961,7 +2961,7 @@
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
     </row>
-    <row r="27" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="22:27">
       <c r="V27" s="12"/>
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
@@ -2969,7 +2969,7 @@
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
     </row>
-    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="22:27">
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
@@ -2995,9 +2995,9 @@
       <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:34">
       <c r="B2" s="22" t="s">
         <v>24</v>
       </c>
@@ -3021,7 +3021,7 @@
       <c r="T2" s="22"/>
       <c r="U2" s="22"/>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:34">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -3044,114 +3044,114 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:34">
       <c r="AH4" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:34">
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:34">
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:34">
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:34">
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:34">
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:34">
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:34">
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:34">
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:34">
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:34">
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:34">
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:34">
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="22:27">
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="22:27">
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="22:27">
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="22:27">
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="22:27">
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="22:27">
       <c r="X28" s="13" t="s">
         <v>39</v>
       </c>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="AA28" s="17"/>
     </row>
-    <row r="29" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="22:27">
       <c r="X29" s="13" t="s">
         <v>40</v>
       </c>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="AA29" s="17"/>
     </row>
-    <row r="32" spans="22:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="22:27">
       <c r="X32" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28">
       <c r="Y33" t="s">
         <v>26</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:28">
       <c r="X34" t="s">
         <v>26</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28">
       <c r="X35" t="s">
         <v>27</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28">
       <c r="X36" t="s">
         <v>29</v>
       </c>
@@ -3222,13 +3222,13 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28">
       <c r="Y37">
         <f>SUM(Y35:Y36)</f>
         <v>2150</v>
       </c>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28">
       <c r="B38" t="s">
         <v>28</v>
       </c>
@@ -3245,6 +3245,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3467,22 +3482,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3499,21 +3516,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjustment to Trade names
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdamV/Desktop/Bachelor/GitHub/Bachelor_Git/TIMES-DE/SuppXLS/Trades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\DTU\TIMES-DE\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAAB9260-654B-8841-9CFE-D39908D95AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D4F3FB-BFF0-4AE1-8B4F-5822891EE7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="444" windowWidth="25704" windowHeight="15948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Data Existing Transmission" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="69">
   <si>
     <t>Year</t>
   </si>
@@ -299,18 +298,6 @@
     <t>FX</t>
   </si>
   <si>
-    <t>TU_ELCC_DE1_DE2_01</t>
-  </si>
-  <si>
-    <t>TU_ELCC_DE1_DE3_01</t>
-  </si>
-  <si>
-    <t>TU_ELCC_DE1_DE4_01</t>
-  </si>
-  <si>
-    <t>TU_ELCC_DE1_DE5_01</t>
-  </si>
-  <si>
     <t>~TFM_DINS</t>
   </si>
   <si>
@@ -330,6 +317,18 @@
   </si>
   <si>
     <t>FLO_MARK</t>
+  </si>
+  <si>
+    <t>TU_ELCC_DE2_DE1_01</t>
+  </si>
+  <si>
+    <t>TU_ELCC_DE3_DE1_01</t>
+  </si>
+  <si>
+    <t>TU_ELCC_DE4_DE1_01</t>
+  </si>
+  <si>
+    <t>TU_ELCC_DE5_DE1_01</t>
   </si>
 </sst>
 </file>
@@ -339,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,10 +594,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1335,7 +1334,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1660,33 +1659,33 @@
   </sheetPr>
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12.6640625" customWidth="1"/>
     <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
-    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1695,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1777,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
         <v>57</v>
@@ -1820,7 +1819,7 @@
       </c>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
@@ -1849,7 +1848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>7</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" s="10" t="s">
         <v>57</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
@@ -1958,7 +1957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +1974,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>9</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>12</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>8</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="10" t="s">
         <v>57</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="22" spans="3:12">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
         <v>41</v>
@@ -2070,7 +2069,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="3:12">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="3:12">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>9</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="25" spans="3:12">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="26" spans="3:12">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>8</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="27" spans="3:12">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" s="10" t="s">
         <v>57</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="28" spans="3:12">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
         <v>41</v>
@@ -2179,7 +2178,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="3:12">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>7</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="3:12">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>9</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="31" spans="3:12">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>12</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="32" spans="3:12">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>8</v>
       </c>
@@ -2241,7 +2240,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="33" spans="3:12">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C33" s="10" t="s">
         <v>57</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="34" spans="3:12">
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C34" s="19"/>
       <c r="D34" s="19" t="s">
         <v>41</v>
@@ -2286,7 +2285,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="3:12">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -2299,11 +2298,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="K35" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="3:12">
+      <c r="K35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>9</v>
       </c>
@@ -2315,10 +2314,10 @@
       </c>
       <c r="K36" s="10" t="str">
         <f>K35</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12">
+        <v>TU_ELCC_DE2_DE1_01</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>12</v>
       </c>
@@ -2330,10 +2329,10 @@
       </c>
       <c r="K37" s="10" t="str">
         <f>K36</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="38" spans="3:12">
+        <v>TU_ELCC_DE2_DE1_01</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>8</v>
       </c>
@@ -2347,10 +2346,10 @@
       <c r="J38" s="8"/>
       <c r="K38" s="10" t="str">
         <f>K37</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
-      </c>
-    </row>
-    <row r="39" spans="3:12">
+        <v>TU_ELCC_DE2_DE1_01</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C39" s="10" t="s">
         <v>11</v>
       </c>
@@ -2370,11 +2369,11 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10" t="str">
         <f>K38</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
+        <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="L39" s="10"/>
     </row>
-    <row r="40" spans="3:12">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>11</v>
       </c>
@@ -2394,11 +2393,11 @@
       <c r="J40" s="9"/>
       <c r="K40" s="10" t="str">
         <f>K35</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
+        <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="L40" s="10"/>
     </row>
-    <row r="41" spans="3:12">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C41" s="19"/>
       <c r="D41" s="19" t="s">
         <v>41</v>
@@ -2414,13 +2413,13 @@
       <c r="J41" s="20"/>
       <c r="K41" s="18" t="str">
         <f>K40</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
+        <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="L41" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="3:12">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>7</v>
       </c>
@@ -2433,11 +2432,11 @@
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="K42" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="3:12">
+      <c r="K42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>9</v>
       </c>
@@ -2449,10 +2448,10 @@
       </c>
       <c r="K43" s="10" t="str">
         <f t="shared" ref="K43:K48" si="5">K42</f>
-        <v>TU_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="44" spans="3:12">
+        <v>TU_ELCC_DE3_DE1_01</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>12</v>
       </c>
@@ -2464,10 +2463,10 @@
       </c>
       <c r="K44" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>TU_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12">
+        <v>TU_ELCC_DE3_DE1_01</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>8</v>
       </c>
@@ -2481,10 +2480,10 @@
       <c r="J45" s="8"/>
       <c r="K45" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>TU_ELCC_DE1_DE3_01</v>
-      </c>
-    </row>
-    <row r="46" spans="3:12">
+        <v>TU_ELCC_DE3_DE1_01</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C46" s="10" t="s">
         <v>11</v>
       </c>
@@ -2504,11 +2503,11 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>TU_ELCC_DE1_DE3_01</v>
+        <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="L46" s="10"/>
     </row>
-    <row r="47" spans="3:12">
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>11</v>
       </c>
@@ -2528,11 +2527,11 @@
       <c r="J47" s="9"/>
       <c r="K47" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>TU_ELCC_DE1_DE3_01</v>
+        <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="L47" s="10"/>
     </row>
-    <row r="48" spans="3:12">
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C48" s="19"/>
       <c r="D48" s="19" t="s">
         <v>41</v>
@@ -2548,13 +2547,13 @@
       <c r="J48" s="20"/>
       <c r="K48" s="18" t="str">
         <f t="shared" si="5"/>
-        <v>TU_ELCC_DE1_DE3_01</v>
+        <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="L48" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:12">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>7</v>
       </c>
@@ -2567,11 +2566,11 @@
       <c r="I49">
         <v>1</v>
       </c>
-      <c r="K49" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="3:12">
+      <c r="K49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>9</v>
       </c>
@@ -2583,10 +2582,10 @@
       </c>
       <c r="K50" s="10" t="str">
         <f t="shared" ref="K50:K55" si="6">K49</f>
-        <v>TU_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="51" spans="3:12">
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>12</v>
       </c>
@@ -2598,10 +2597,10 @@
       </c>
       <c r="K51" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>TU_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="52" spans="3:12">
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>8</v>
       </c>
@@ -2614,10 +2613,10 @@
       <c r="J52" s="8"/>
       <c r="K52" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>TU_ELCC_DE1_DE4_01</v>
-      </c>
-    </row>
-    <row r="53" spans="3:12">
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C53" s="10" t="s">
         <v>11</v>
       </c>
@@ -2636,11 +2635,11 @@
       <c r="J53" s="10"/>
       <c r="K53" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>TU_ELCC_DE1_DE4_01</v>
+        <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="L53" s="10"/>
     </row>
-    <row r="54" spans="3:12">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>11</v>
       </c>
@@ -2659,11 +2658,11 @@
       <c r="J54" s="9"/>
       <c r="K54" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>TU_ELCC_DE1_DE4_01</v>
+        <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="L54" s="10"/>
     </row>
-    <row r="55" spans="3:12">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C55" s="19"/>
       <c r="D55" s="19" t="s">
         <v>41</v>
@@ -2678,13 +2677,13 @@
       <c r="J55" s="20"/>
       <c r="K55" s="18" t="str">
         <f t="shared" si="6"/>
-        <v>TU_ELCC_DE1_DE4_01</v>
+        <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="L55" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="3:12">
+    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>7</v>
       </c>
@@ -2697,11 +2696,11 @@
       <c r="J56">
         <v>1</v>
       </c>
-      <c r="K56" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="3:12">
+      <c r="K56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>9</v>
       </c>
@@ -2713,10 +2712,10 @@
       </c>
       <c r="K57" s="10" t="str">
         <f t="shared" ref="K57:K62" si="7">K56</f>
-        <v>TU_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="58" spans="3:12">
+        <v>TU_ELCC_DE5_DE1_01</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>12</v>
       </c>
@@ -2728,10 +2727,10 @@
       </c>
       <c r="K58" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>TU_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="59" spans="3:12">
+        <v>TU_ELCC_DE5_DE1_01</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>8</v>
       </c>
@@ -2743,10 +2742,10 @@
       </c>
       <c r="K59" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>TU_ELCC_DE1_DE5_01</v>
-      </c>
-    </row>
-    <row r="60" spans="3:12">
+        <v>TU_ELCC_DE5_DE1_01</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C60" s="10" t="s">
         <v>11</v>
       </c>
@@ -2764,11 +2763,11 @@
       </c>
       <c r="K60" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>TU_ELCC_DE1_DE5_01</v>
+        <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="L60" s="10"/>
     </row>
-    <row r="61" spans="3:12">
+    <row r="61" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2786,11 +2785,11 @@
       </c>
       <c r="K61" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>TU_ELCC_DE1_DE5_01</v>
+        <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="L61" s="10"/>
     </row>
-    <row r="62" spans="3:12">
+    <row r="62" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C62" s="19"/>
       <c r="D62" s="19" t="s">
         <v>41</v>
@@ -2804,7 +2803,7 @@
       </c>
       <c r="K62" s="18" t="str">
         <f t="shared" si="7"/>
-        <v>TU_ELCC_DE1_DE5_01</v>
+        <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="L62" s="18" t="s">
         <v>45</v>
@@ -2823,19 +2822,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0360F3E-BECD-4B31-BDCB-111249D854EE}">
   <dimension ref="B3:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2846,15 +2845,15 @@
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>3</v>
@@ -2870,129 +2869,129 @@
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="30">
+      <c r="C5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="29">
         <v>2010</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <v>0.1</v>
       </c>
       <c r="J5">
         <v>0.10686678676759548</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="30" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="30">
+      <c r="C6" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="29">
         <v>2010</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <v>0.1</v>
       </c>
       <c r="J6">
         <v>2.4997560823677975E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="30" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="30">
+      <c r="C7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="29">
         <v>2010</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <v>0.1</v>
       </c>
       <c r="J7">
         <v>2.202997304070314E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="30" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="30">
+      <c r="C8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="29">
         <v>2010</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <v>0.1</v>
       </c>
       <c r="J8">
         <v>2.0027248218821018E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
-        <f>ELC_TRADE!K39</f>
-        <v>TU_ELCC_DE1_DE2_01</v>
+        <f>B5</f>
+        <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G9">
         <v>2050</v>
@@ -3001,22 +3000,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
-        <f>ELC_TRADE!K46</f>
-        <v>TU_ELCC_DE1_DE3_01</v>
+        <f t="shared" ref="B10:B16" si="0">B6</f>
+        <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G10">
         <v>2050</v>
@@ -3025,22 +3024,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
-        <f>ELC_TRADE!K53</f>
-        <v>TU_ELCC_DE1_DE4_01</v>
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G11">
         <v>2050</v>
@@ -3049,22 +3048,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
-        <f>ELC_TRADE!K60</f>
-        <v>TU_ELCC_DE1_DE5_01</v>
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G12">
         <v>2050</v>
@@ -3073,21 +3072,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" t="s">
-        <v>58</v>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -3096,21 +3096,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>59</v>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3119,21 +3120,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
-      <c r="B15" t="s">
-        <v>60</v>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -3142,21 +3144,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
-        <v>61</v>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3182,20 +3185,20 @@
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="24" max="24" width="10.6640625" customWidth="1"/>
     <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.5" customWidth="1"/>
-    <col min="27" max="27" width="16.5" customWidth="1"/>
+    <col min="26" max="26" width="17.44140625" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="20">
+    <row r="1" spans="2:27" ht="19.8" x14ac:dyDescent="0.4">
       <c r="B1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:27">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="X2" t="s">
         <v>23</v>
       </c>
@@ -3203,7 +3206,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:27">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="X3" t="s">
         <v>14</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:27">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="X4" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:27">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V5" t="s">
         <v>15</v>
       </c>
@@ -3230,7 +3233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:27">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V6" t="s">
         <v>20</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="2:27">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V7" t="s">
         <v>20</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:27">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V9" t="s">
         <v>38</v>
       </c>
@@ -3276,12 +3279,12 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:27">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="W12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:27">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="W13" t="s">
         <v>29</v>
       </c>
@@ -3289,12 +3292,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:27">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="W14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:27">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V15" s="12"/>
       <c r="W15" s="12">
         <f>Z9/2</f>
@@ -3308,7 +3311,7 @@
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
     </row>
-    <row r="16" spans="2:27">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
@@ -3316,7 +3319,7 @@
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
     </row>
-    <row r="17" spans="22:27">
+    <row r="17" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
@@ -3324,7 +3327,7 @@
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
     </row>
-    <row r="18" spans="22:27">
+    <row r="18" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
@@ -3332,7 +3335,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
     </row>
-    <row r="19" spans="22:27">
+    <row r="19" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
@@ -3340,7 +3343,7 @@
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
     </row>
-    <row r="20" spans="22:27">
+    <row r="20" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
@@ -3348,7 +3351,7 @@
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
     </row>
-    <row r="21" spans="22:27">
+    <row r="21" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
@@ -3356,7 +3359,7 @@
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
     </row>
-    <row r="22" spans="22:27">
+    <row r="22" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
@@ -3364,7 +3367,7 @@
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
     </row>
-    <row r="23" spans="22:27">
+    <row r="23" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
@@ -3372,7 +3375,7 @@
       <c r="Z23" s="12"/>
       <c r="AA23" s="12"/>
     </row>
-    <row r="24" spans="22:27">
+    <row r="24" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V24" s="12"/>
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
@@ -3380,7 +3383,7 @@
       <c r="Z24" s="12"/>
       <c r="AA24" s="12"/>
     </row>
-    <row r="25" spans="22:27">
+    <row r="25" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
@@ -3388,7 +3391,7 @@
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
     </row>
-    <row r="26" spans="22:27">
+    <row r="26" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
@@ -3396,7 +3399,7 @@
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
     </row>
-    <row r="27" spans="22:27">
+    <row r="27" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V27" s="12"/>
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
@@ -3404,7 +3407,7 @@
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
     </row>
-    <row r="28" spans="22:27">
+    <row r="28" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
@@ -3430,163 +3433,163 @@
       <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:34">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="M2" s="29" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="M2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-    </row>
-    <row r="3" spans="2:34">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
       <c r="AH3" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:34">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
       <c r="AH4" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:34">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="2:34">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="2:34">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="2:34">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="2:34">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="2:34">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="2:34">
+    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="2:34">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="2:34">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" spans="2:34">
+    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="2:34">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="2:34">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="22:27">
+    <row r="17" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="22:27">
+    <row r="18" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="22:27">
+    <row r="19" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="22:27">
+    <row r="20" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" spans="22:27">
+    <row r="21" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="28" spans="22:27">
+    <row r="28" spans="22:27" x14ac:dyDescent="0.3">
       <c r="X28" s="13" t="s">
         <v>39</v>
       </c>
@@ -3598,7 +3601,7 @@
       </c>
       <c r="AA28" s="17"/>
     </row>
-    <row r="29" spans="22:27">
+    <row r="29" spans="22:27" x14ac:dyDescent="0.3">
       <c r="X29" s="13" t="s">
         <v>40</v>
       </c>
@@ -3610,12 +3613,12 @@
       </c>
       <c r="AA29" s="17"/>
     </row>
-    <row r="32" spans="22:27">
+    <row r="32" spans="22:27" x14ac:dyDescent="0.3">
       <c r="X32" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:28">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="Y33" t="s">
         <v>26</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:28">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.3">
       <c r="X34" t="s">
         <v>26</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="35" spans="2:28">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="X35" t="s">
         <v>27</v>
       </c>
@@ -3649,7 +3652,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="2:28">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
       <c r="X36" t="s">
         <v>29</v>
       </c>
@@ -3657,13 +3660,13 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="37" spans="2:28">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
       <c r="Y37">
         <f>SUM(Y35:Y36)</f>
         <v>2150</v>
       </c>
     </row>
-    <row r="38" spans="2:28">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>28</v>
       </c>
@@ -3686,6 +3689,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3908,15 +3920,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
   <ds:schemaRefs>
@@ -3927,6 +3930,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3943,12 +3954,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove upper limit on elcc to DE1 from other regions
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\Trades\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14970B43-A6D9-4281-90CC-C5C09FA76156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17016" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Data New Transmission" sheetId="3" r:id="rId3"/>
     <sheet name="Data Existing Transmission" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,13 +28,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{29A67EE3-41B7-4DDB-B48A-850B5DE5423E}">
+    <comment ref="H3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -67,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="1" shapeId="0" xr:uid="{BCDEF17F-9BC4-494F-8612-27052E0883A3}">
+    <comment ref="I3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -80,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="J3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -98,12 +92,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{24D2D3A7-648A-4A4B-873E-EAE23E89B458}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="68">
   <si>
     <t>Year</t>
   </si>
@@ -331,7 +325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -553,7 +547,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,7 +561,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -597,17 +590,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma0 - Type3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Fixed2 - Type2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Bad 2" xfId="1"/>
+    <cellStyle name="Comma0 - Type3" xfId="2"/>
+    <cellStyle name="Fixed2 - Type2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Percen - Type1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Valore valido" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 10" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7"/>
+    <cellStyle name="Percen - Type1" xfId="8"/>
+    <cellStyle name="Percent 2" xfId="9"/>
+    <cellStyle name="Valore valido" xfId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,7 +635,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -721,7 +714,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -819,7 +812,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -863,7 +856,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -907,7 +900,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -951,7 +944,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1000,7 +993,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1054,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1122,7 +1115,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1252,7 +1245,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1301,7 +1294,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,9 +1324,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1371,9 +1364,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1406,26 +1399,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,26 +1434,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1650,39 +1609,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.6328125" customWidth="1"/>
-    <col min="11" max="11" width="23.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19.453125" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1727,7 +1686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -1740,11 +1699,11 @@
       <c r="H5">
         <v>0.97</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -1754,12 +1713,12 @@
       <c r="H6">
         <v>0.92</v>
       </c>
-      <c r="K6" s="10" t="str">
+      <c r="K6" s="9" t="str">
         <f>K5</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>12</v>
       </c>
@@ -1769,12 +1728,12 @@
       <c r="H7">
         <v>50</v>
       </c>
-      <c r="K7" s="10" t="str">
+      <c r="K7" s="9" t="str">
         <f>K6</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -1786,66 +1745,66 @@
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="10" t="str">
+      <c r="K8" s="9" t="str">
         <f t="shared" ref="K8:K9" si="0">K7</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
+    <row r="9" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E9">
         <v>2010</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>8634</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>8634</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10" t="str">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="20">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <f>'Data New Transmission'!W15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="18" t="str">
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="17" t="str">
         <f>K9</f>
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="17" t="s">
         <v>45</v>
       </c>
       <c r="N10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>7</v>
       </c>
@@ -1858,11 +1817,11 @@
       <c r="J11">
         <v>0.97</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -1872,12 +1831,12 @@
       <c r="J12">
         <v>0.92</v>
       </c>
-      <c r="K12" s="10" t="str">
+      <c r="K12" s="9" t="str">
         <f>K11</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -1887,12 +1846,12 @@
       <c r="J13">
         <v>50</v>
       </c>
-      <c r="K13" s="10" t="str">
+      <c r="K13" s="9" t="str">
         <f>K12</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -1902,59 +1861,59 @@
       <c r="J14" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K14" s="10" t="str">
+      <c r="K14" s="9" t="str">
         <f t="shared" ref="K14" si="1">K13</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C15" s="10" t="s">
+    <row r="15" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E15">
         <v>2010</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>3010</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>3010</v>
       </c>
-      <c r="K15" s="10" t="str">
+      <c r="K15" s="9" t="str">
         <f>K14</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
+    <row r="16" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="20">
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="20">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="K16" s="18" t="str">
+      <c r="K16" s="17" t="str">
         <f>K15</f>
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="L16" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -1967,11 +1926,11 @@
       <c r="I17">
         <v>0.97</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>9</v>
       </c>
@@ -1981,12 +1940,12 @@
       <c r="I18">
         <v>0.92</v>
       </c>
-      <c r="K18" s="10" t="str">
+      <c r="K18" s="9" t="str">
         <f>K17</f>
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>12</v>
       </c>
@@ -1996,12 +1955,12 @@
       <c r="I19">
         <v>50</v>
       </c>
-      <c r="K19" s="10" t="str">
+      <c r="K19" s="9" t="str">
         <f>K18</f>
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>8</v>
       </c>
@@ -2012,61 +1971,61 @@
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="J20" s="8"/>
-      <c r="K20" s="10" t="str">
+      <c r="K20" s="9" t="str">
         <f t="shared" ref="K20" si="2">K19</f>
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C21" s="10" t="s">
+    <row r="21" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E21">
         <v>2010</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="20">
         <f>14416</f>
         <v>14416</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="20">
         <f>14416</f>
         <v>14416</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10" t="str">
+      <c r="J21" s="9"/>
+      <c r="K21" s="9" t="str">
         <f>K20</f>
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C22" s="19"/>
-      <c r="D22" s="19" t="s">
+    <row r="22" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="20">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="I22" s="20">
+      <c r="I22" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="18" t="str">
+      <c r="J22" s="19"/>
+      <c r="K22" s="17" t="str">
         <f>K21</f>
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
-      <c r="L22" s="18" t="s">
+      <c r="L22" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -2079,11 +2038,11 @@
       <c r="J23">
         <v>0.97</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>9</v>
       </c>
@@ -2093,12 +2052,12 @@
       <c r="J24">
         <v>0.92</v>
       </c>
-      <c r="K24" s="10" t="str">
+      <c r="K24" s="9" t="str">
         <f>K23</f>
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -2108,12 +2067,12 @@
       <c r="J25">
         <v>50</v>
       </c>
-      <c r="K25" s="10" t="str">
+      <c r="K25" s="9" t="str">
         <f>K24</f>
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>8</v>
       </c>
@@ -2123,59 +2082,59 @@
       <c r="J26" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K26" s="10" t="str">
+      <c r="K26" s="9" t="str">
         <f t="shared" ref="K26" si="3">K25</f>
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C27" s="10" t="s">
+    <row r="27" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E27">
         <v>2010</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="20">
         <v>6020</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21">
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>6020</v>
       </c>
-      <c r="K27" s="10" t="str">
+      <c r="K27" s="9" t="str">
         <f>K26</f>
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+    <row r="28" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="20">
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="20">
+      <c r="I28" s="17"/>
+      <c r="J28" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="K28" s="18" t="str">
+      <c r="K28" s="17" t="str">
         <f>K27</f>
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
-      <c r="L28" s="18" t="s">
+      <c r="L28" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>7</v>
       </c>
@@ -2188,11 +2147,11 @@
       <c r="J29">
         <v>0.97</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
         <v>9</v>
       </c>
@@ -2202,12 +2161,12 @@
       <c r="J30">
         <v>0.92</v>
       </c>
-      <c r="K30" s="10" t="str">
+      <c r="K30" s="9" t="str">
         <f>K29</f>
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>12</v>
       </c>
@@ -2217,12 +2176,12 @@
       <c r="J31">
         <v>50</v>
       </c>
-      <c r="K31" s="10" t="str">
+      <c r="K31" s="9" t="str">
         <f>K30</f>
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>8</v>
       </c>
@@ -2232,57 +2191,57 @@
       <c r="J32" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K32" s="10" t="str">
+      <c r="K32" s="9" t="str">
         <f t="shared" ref="K32" si="4">K31</f>
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C33" s="10" t="s">
+    <row r="33" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E33">
         <v>2010</v>
       </c>
-      <c r="I33" s="21">
+      <c r="I33" s="20">
         <v>3010</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="20">
         <v>3010</v>
       </c>
-      <c r="K33" s="10" t="str">
+      <c r="K33" s="9" t="str">
         <f>K32</f>
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
+    <row r="34" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C34" s="18"/>
+      <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="I34" s="20">
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="I34" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="J34" s="20">
+      <c r="J34" s="19">
         <f>'Data New Transmission'!$X$15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="K34" s="18" t="str">
+      <c r="K34" s="17" t="str">
         <f>K33</f>
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
-      <c r="L34" s="18" t="s">
+      <c r="L34" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -2299,7 +2258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>9</v>
       </c>
@@ -2309,12 +2268,12 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="K36" s="10" t="str">
+      <c r="K36" s="9" t="str">
         <f>K35</f>
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>12</v>
       </c>
@@ -2324,12 +2283,12 @@
       <c r="G37">
         <v>100</v>
       </c>
-      <c r="K37" s="10" t="str">
+      <c r="K37" s="9" t="str">
         <f>K36</f>
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>8</v>
       </c>
@@ -2341,468 +2300,282 @@
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="10" t="str">
+      <c r="K38" s="9" t="str">
         <f>K37</f>
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C39" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39">
-        <v>2010</v>
-      </c>
-      <c r="F39" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="G39" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10" t="str">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="18"/>
+      <c r="D39" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="19">
+        <v>0</v>
+      </c>
+      <c r="G39" s="19">
+        <v>0</v>
+      </c>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="17" t="str">
         <f>K38</f>
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
-      <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
+      <c r="L39" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="9">
-        <v>5</v>
-      </c>
-      <c r="G40" s="9">
-        <v>5</v>
-      </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="10" t="str">
-        <f>K35</f>
-        <v>TU_ELCC_DE2_DE1_01</v>
-      </c>
-      <c r="L40" s="10"/>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C41" s="19"/>
-      <c r="D41" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="20">
-        <v>0</v>
-      </c>
-      <c r="G41" s="20">
-        <v>0</v>
-      </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="18" t="str">
-        <f>K40</f>
-        <v>TU_ELCC_DE2_DE1_01</v>
-      </c>
-      <c r="L41" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
+        <v>2010</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="K41" s="9" t="str">
+        <f t="shared" ref="K41:K43" si="5">K40</f>
+        <v>TU_ELCC_DE3_DE1_01</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42">
-        <v>2010</v>
+        <v>12</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="K42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="K43" s="10" t="str">
-        <f t="shared" ref="K43:K48" si="5">K42</f>
-        <v>TU_ELCC_DE3_DE1_01</v>
-      </c>
-    </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44">
         <v>100</v>
       </c>
-      <c r="H44">
-        <v>100</v>
-      </c>
-      <c r="K44" s="10" t="str">
+      <c r="K42" s="9" t="str">
         <f t="shared" si="5"/>
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D45" t="s">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F43" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H43" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="10" t="str">
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="9" t="str">
         <f t="shared" si="5"/>
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C46" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C44" s="18"/>
+      <c r="D44" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="19">
+        <v>0</v>
+      </c>
+      <c r="H44" s="19">
+        <v>0</v>
+      </c>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="17" t="str">
+        <f>K43</f>
+        <v>TU_ELCC_DE3_DE1_01</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45">
         <v>2010</v>
       </c>
-      <c r="F46" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="H46" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>TU_ELCC_DE3_DE1_01</v>
-      </c>
-      <c r="L46" s="10"/>
-    </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="K46" s="9" t="str">
+        <f t="shared" ref="K46:K48" si="6">K45</f>
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47">
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+      <c r="I47">
+        <v>100</v>
+      </c>
+      <c r="K47" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="I48" s="8">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J48" s="8"/>
+      <c r="K48" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C49" s="18"/>
+      <c r="D49" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="19">
         <v>0</v>
       </c>
-      <c r="F47" s="9">
-        <v>5</v>
-      </c>
-      <c r="H47" s="9">
-        <v>5</v>
-      </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>TU_ELCC_DE3_DE1_01</v>
-      </c>
-      <c r="L47" s="10"/>
-    </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C48" s="19"/>
-      <c r="D48" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="18"/>
-      <c r="F48" s="20">
+      <c r="I49" s="19">
         <v>0</v>
       </c>
-      <c r="H48" s="20">
-        <v>0</v>
-      </c>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>TU_ELCC_DE3_DE1_01</v>
-      </c>
-      <c r="L48" s="18" t="s">
+      <c r="J49" s="19"/>
+      <c r="K49" s="17" t="str">
+        <f>K48</f>
+        <v>TU_ELCC_DE4_DE1_01</v>
+      </c>
+      <c r="L49" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D49" t="s">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
         <v>7</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>2010</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-      <c r="K49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D50" t="s">
-        <v>9</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>1</v>
       </c>
-      <c r="K50" s="10" t="str">
-        <f t="shared" ref="K50:K55" si="6">K49</f>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-    </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="K50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" s="9" t="str">
+        <f t="shared" ref="K51:K53" si="7">K50</f>
+        <v>TU_ELCC_DE5_DE1_01</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="F51">
+      <c r="F52">
         <v>100</v>
       </c>
-      <c r="I51">
+      <c r="J52">
         <v>100</v>
       </c>
-      <c r="K51" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-    </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="I52" s="8">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="J52" s="8"/>
-      <c r="K52" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-    </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C53" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53">
-        <v>2010</v>
-      </c>
-      <c r="F53" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="I53" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-      <c r="L53" s="10"/>
-    </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54" s="9">
-        <v>5</v>
-      </c>
-      <c r="I54" s="9">
-        <v>5</v>
-      </c>
-      <c r="J54" s="9"/>
-      <c r="K54" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-      <c r="L54" s="10"/>
-    </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C55" s="19"/>
-      <c r="D55" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="20">
-        <v>0</v>
-      </c>
-      <c r="I55" s="20">
-        <v>0</v>
-      </c>
-      <c r="J55" s="20"/>
-      <c r="K55" s="18" t="str">
-        <f t="shared" si="6"/>
-        <v>TU_ELCC_DE4_DE1_01</v>
-      </c>
-      <c r="L55" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56">
-        <v>2010</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="J56">
-        <v>1</v>
-      </c>
-      <c r="K56" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-      <c r="K57" s="10" t="str">
-        <f t="shared" ref="K57:K62" si="7">K56</f>
-        <v>TU_ELCC_DE5_DE1_01</v>
-      </c>
-    </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58">
-        <v>100</v>
-      </c>
-      <c r="J58">
-        <v>100</v>
-      </c>
-      <c r="K58" s="10" t="str">
+      <c r="K52" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="D59" t="s">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
         <v>8</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F53" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J53" s="8">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K59" s="10" t="str">
+      <c r="K53" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C60" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60">
-        <v>2010</v>
-      </c>
-      <c r="F60" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="J60" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="K60" s="10" t="str">
-        <f t="shared" si="7"/>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C54" s="18"/>
+      <c r="D54" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="17"/>
+      <c r="F54" s="19">
+        <v>0</v>
+      </c>
+      <c r="J54" s="19">
+        <v>0</v>
+      </c>
+      <c r="K54" s="17" t="str">
+        <f>K53</f>
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
-      <c r="L60" s="10"/>
-    </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C61" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61" s="9">
-        <v>5</v>
-      </c>
-      <c r="J61" s="9">
-        <v>5</v>
-      </c>
-      <c r="K61" s="10" t="str">
-        <f t="shared" si="7"/>
-        <v>TU_ELCC_DE5_DE1_01</v>
-      </c>
-      <c r="L61" s="10"/>
-    </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C62" s="19"/>
-      <c r="D62" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="18"/>
-      <c r="F62" s="20">
-        <v>0</v>
-      </c>
-      <c r="J62" s="20">
-        <v>0</v>
-      </c>
-      <c r="K62" s="18" t="str">
-        <f t="shared" si="7"/>
-        <v>TU_ELCC_DE5_DE1_01</v>
-      </c>
-      <c r="L62" s="18" t="s">
+      <c r="L54" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2816,79 +2589,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0360F3E-BECD-4B31-BDCB-111249D854EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="27" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>2010</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="28">
         <v>0.1</v>
       </c>
       <c r="J5">
@@ -2896,25 +2669,25 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>2010</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <v>0.1</v>
       </c>
       <c r="J6">
@@ -2922,25 +2695,25 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <v>2010</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <v>0.1</v>
       </c>
       <c r="J7">
@@ -2948,25 +2721,25 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <v>2010</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="28">
         <v>0.1</v>
       </c>
       <c r="J8">
@@ -3172,7 +2945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3182,20 +2955,20 @@
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="24" max="24" width="10.6328125" customWidth="1"/>
-    <col min="25" max="25" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.453125" customWidth="1"/>
-    <col min="27" max="27" width="16.453125" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.44140625" customWidth="1"/>
+    <col min="27" max="27" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X2" t="s">
         <v>23</v>
       </c>
@@ -3203,7 +2976,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X3" t="s">
         <v>14</v>
       </c>
@@ -3211,7 +2984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X4" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +2995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="V5" t="s">
         <v>15</v>
       </c>
@@ -3230,7 +3003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="V6" t="s">
         <v>20</v>
       </c>
@@ -3244,7 +3017,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="V7" t="s">
         <v>20</v>
       </c>
@@ -3258,7 +3031,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="V9" t="s">
         <v>38</v>
       </c>
@@ -3276,12 +3049,12 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="W12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="W13" t="s">
         <v>29</v>
       </c>
@@ -3289,128 +3062,128 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
       <c r="W14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="V15" s="12"/>
-      <c r="W15" s="12">
+    <row r="15" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V15" s="11"/>
+      <c r="W15" s="11">
         <f>Z9/2</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="X15" s="12">
+      <c r="X15" s="11">
         <f>W15</f>
         <v>0.26750000000000002</v>
       </c>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-    </row>
-    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-    </row>
-    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="12"/>
-    </row>
-    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-    </row>
-    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-    </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12"/>
-    </row>
-    <row r="22" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-    </row>
-    <row r="23" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-    </row>
-    <row r="24" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="12"/>
-    </row>
-    <row r="25" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
-    </row>
-    <row r="26" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-    </row>
-    <row r="27" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-    </row>
-    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+    </row>
+    <row r="16" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+    </row>
+    <row r="17" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+    </row>
+    <row r="18" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+    </row>
+    <row r="19" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+    </row>
+    <row r="20" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+    </row>
+    <row r="21" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+    </row>
+    <row r="22" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+    </row>
+    <row r="23" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+    </row>
+    <row r="24" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+    </row>
+    <row r="25" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+    </row>
+    <row r="26" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+    </row>
+    <row r="27" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+    </row>
+    <row r="28" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3420,7 +3193,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3430,192 +3203,192 @@
       <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="M2" s="30" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="M2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-    </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="AH3" s="15" t="s">
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="AH3" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="AH4" s="16" t="s">
+    <row r="4" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="AH4" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-    </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-    </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.35">
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-    </row>
-    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-    </row>
-    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-    </row>
-    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-    </row>
-    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
-    </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-    </row>
-    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="X28" s="13" t="s">
+    <row r="5" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+    </row>
+    <row r="6" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+    </row>
+    <row r="7" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+    </row>
+    <row r="8" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+    </row>
+    <row r="9" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+    </row>
+    <row r="10" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+    </row>
+    <row r="11" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+    </row>
+    <row r="12" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+    </row>
+    <row r="13" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+    </row>
+    <row r="14" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+    </row>
+    <row r="15" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+    </row>
+    <row r="16" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+    </row>
+    <row r="17" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+    </row>
+    <row r="18" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+    </row>
+    <row r="19" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+    </row>
+    <row r="20" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+    </row>
+    <row r="21" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+    </row>
+    <row r="28" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="X28" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Y28" s="17" t="s">
+      <c r="Y28" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="Z28" s="17" t="s">
+      <c r="Z28" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="AA28" s="17"/>
-    </row>
-    <row r="29" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="X29" s="13" t="s">
+      <c r="AA28" s="16"/>
+    </row>
+    <row r="29" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="X29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Y29" s="17" t="s">
+      <c r="Y29" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="Z29" s="17" t="s">
+      <c r="Z29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AA29" s="17"/>
-    </row>
-    <row r="32" spans="22:27" x14ac:dyDescent="0.35">
-      <c r="X32" s="14" t="s">
+      <c r="AA29" s="16"/>
+    </row>
+    <row r="32" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="X32" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="Y33" t="s">
         <v>26</v>
       </c>
@@ -3626,7 +3399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X34" t="s">
         <v>26</v>
       </c>
@@ -3641,7 +3414,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X35" t="s">
         <v>27</v>
       </c>
@@ -3649,7 +3422,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="X36" t="s">
         <v>29</v>
       </c>
@@ -3657,13 +3430,13 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="Y37">
         <f>SUM(Y35:Y36)</f>
         <v>2150</v>
       </c>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Nu capacity i PJ
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\Trades\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C28E61-0999-4C52-8041-C8EA40BCBD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17016" windowHeight="10416"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="Data New Transmission" sheetId="3" r:id="rId3"/>
     <sheet name="Data Existing Transmission" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -21,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,13 +35,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1">
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="1">
+    <comment ref="I3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1">
+    <comment ref="J3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -92,12 +99,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -325,7 +332,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -590,17 +597,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Bad 2" xfId="1"/>
-    <cellStyle name="Comma0 - Type3" xfId="2"/>
-    <cellStyle name="Fixed2 - Type2" xfId="3"/>
+    <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma0 - Type3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Fixed2 - Type2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="4"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7"/>
-    <cellStyle name="Percen - Type1" xfId="8"/>
-    <cellStyle name="Percent 2" xfId="9"/>
-    <cellStyle name="Valore valido" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Percen - Type1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Valore valido" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -635,7 +642,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -714,7 +721,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -812,7 +819,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +863,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -900,7 +907,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -944,7 +951,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -993,7 +1000,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1054,7 +1061,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1115,7 +1122,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1245,7 +1252,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1294,7 +1301,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,9 +1331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1364,9 +1371,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1399,9 +1406,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1434,9 +1458,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1609,39 +1650,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="23.36328125" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" customWidth="1"/>
+    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1686,7 +1727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>7</v>
       </c>
@@ -1703,7 +1744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1759,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>12</v>
       </c>
@@ -1733,7 +1774,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>8</v>
       </c>
@@ -1750,7 +1791,7 @@
         <v>TB_ELCC_DE2_DE3_01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
         <v>11</v>
@@ -1775,7 +1816,7 @@
       </c>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18" t="s">
@@ -1804,7 +1845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>7</v>
       </c>
@@ -1821,7 +1862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1877,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -1851,7 +1892,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -1866,7 +1907,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1928,7 @@
         <v>TB_ELCC_DE2_DE5_01</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18" t="s">
@@ -1913,7 +1954,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1971,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>9</v>
       </c>
@@ -1945,7 +1986,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="19" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>12</v>
       </c>
@@ -1960,7 +2001,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="20" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>8</v>
       </c>
@@ -1976,7 +2017,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="21" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C21" s="9" t="s">
         <v>11</v>
       </c>
@@ -2000,7 +2041,7 @@
         <v>TB_ELCC_DE3_DE4_01</v>
       </c>
     </row>
-    <row r="22" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="18"/>
       <c r="D22" s="18" t="s">
         <v>41</v>
@@ -2025,7 +2066,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -2042,7 +2083,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2098,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="25" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -2072,7 +2113,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="26" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>8</v>
       </c>
@@ -2087,7 +2128,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="27" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="9" t="s">
         <v>11</v>
       </c>
@@ -2109,7 +2150,7 @@
         <v>TB_ELCC_DE3_DE5_01</v>
       </c>
     </row>
-    <row r="28" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
         <v>41</v>
@@ -2134,7 +2175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>7</v>
       </c>
@@ -2151,7 +2192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
         <v>9</v>
       </c>
@@ -2166,7 +2207,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="31" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>12</v>
       </c>
@@ -2181,7 +2222,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="32" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>8</v>
       </c>
@@ -2196,7 +2237,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="33" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C33" s="9" t="s">
         <v>11</v>
       </c>
@@ -2217,7 +2258,7 @@
         <v>TB_ELCC_DE4_DE5_01</v>
       </c>
     </row>
-    <row r="34" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C34" s="18"/>
       <c r="D34" s="18" t="s">
         <v>41</v>
@@ -2241,7 +2282,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -2258,7 +2299,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>9</v>
       </c>
@@ -2273,7 +2314,7 @@
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="37" spans="3:12" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>12</v>
       </c>
@@ -2288,7 +2329,7 @@
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>8</v>
       </c>
@@ -2305,17 +2346,17 @@
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C39" s="18"/>
       <c r="D39" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="G39" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
@@ -2327,7 +2368,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>7</v>
       </c>
@@ -2344,7 +2385,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>9</v>
       </c>
@@ -2359,7 +2400,7 @@
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>12</v>
       </c>
@@ -2374,7 +2415,7 @@
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
         <v>8</v>
       </c>
@@ -2391,17 +2432,17 @@
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C44" s="18"/>
       <c r="D44" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="H44" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
@@ -2413,7 +2454,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>7</v>
       </c>
@@ -2430,7 +2471,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>9</v>
       </c>
@@ -2445,7 +2486,7 @@
         <v>TU_ELCC_DE4_DE1_01</v>
       </c>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D47" t="s">
         <v>12</v>
       </c>
@@ -2460,7 +2501,7 @@
         <v>TU_ELCC_DE4_DE1_01</v>
       </c>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D48" t="s">
         <v>8</v>
       </c>
@@ -2476,17 +2517,17 @@
         <v>TU_ELCC_DE4_DE1_01</v>
       </c>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C49" s="18"/>
       <c r="D49" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I49" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="J49" s="19"/>
       <c r="K49" s="17" t="str">
@@ -2497,7 +2538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D50" t="s">
         <v>7</v>
       </c>
@@ -2514,7 +2555,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D51" t="s">
         <v>9</v>
       </c>
@@ -2529,7 +2570,7 @@
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
     </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D52" t="s">
         <v>12</v>
       </c>
@@ -2544,7 +2585,7 @@
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
       <c r="D53" t="s">
         <v>8</v>
       </c>
@@ -2559,17 +2600,17 @@
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C54" s="18"/>
       <c r="D54" s="18" t="s">
         <v>41</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="J54" s="19">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="K54" s="17" t="str">
         <f>K53</f>
@@ -2589,17 +2630,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
@@ -2945,7 +2986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2955,12 +2996,12 @@
       <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="24" max="24" width="10.6640625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.44140625" customWidth="1"/>
-    <col min="27" max="27" width="16.44140625" customWidth="1"/>
+    <col min="24" max="24" width="10.6328125" customWidth="1"/>
+    <col min="25" max="25" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.453125" customWidth="1"/>
+    <col min="27" max="27" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="19.5" x14ac:dyDescent="0.45">
@@ -2968,7 +3009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
       <c r="X2" t="s">
         <v>23</v>
       </c>
@@ -2976,7 +3017,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
       <c r="X3" t="s">
         <v>14</v>
       </c>
@@ -2984,7 +3025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.35">
       <c r="X4" t="s">
         <v>18</v>
       </c>
@@ -2995,7 +3036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V5" t="s">
         <v>15</v>
       </c>
@@ -3003,7 +3044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V6" t="s">
         <v>20</v>
       </c>
@@ -3017,7 +3058,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V7" t="s">
         <v>20</v>
       </c>
@@ -3031,7 +3072,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V9" t="s">
         <v>38</v>
       </c>
@@ -3049,12 +3090,12 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
       <c r="W12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
       <c r="W13" t="s">
         <v>29</v>
       </c>
@@ -3062,12 +3103,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
       <c r="W14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V15" s="11"/>
       <c r="W15" s="11">
         <f>Z9/2</f>
@@ -3081,7 +3122,7 @@
       <c r="Z15" s="11"/>
       <c r="AA15" s="11"/>
     </row>
-    <row r="16" spans="2:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
@@ -3089,7 +3130,7 @@
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
     </row>
-    <row r="17" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
@@ -3097,7 +3138,7 @@
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
     </row>
-    <row r="18" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
@@ -3105,7 +3146,7 @@
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
     </row>
-    <row r="19" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
@@ -3113,7 +3154,7 @@
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
     </row>
-    <row r="20" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
@@ -3121,7 +3162,7 @@
       <c r="Z20" s="11"/>
       <c r="AA20" s="11"/>
     </row>
-    <row r="21" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
@@ -3129,7 +3170,7 @@
       <c r="Z21" s="11"/>
       <c r="AA21" s="11"/>
     </row>
-    <row r="22" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V22" s="11"/>
       <c r="W22" s="11"/>
       <c r="X22" s="11"/>
@@ -3137,7 +3178,7 @@
       <c r="Z22" s="11"/>
       <c r="AA22" s="11"/>
     </row>
-    <row r="23" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="23" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
       <c r="X23" s="11"/>
@@ -3145,7 +3186,7 @@
       <c r="Z23" s="11"/>
       <c r="AA23" s="11"/>
     </row>
-    <row r="24" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="24" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
       <c r="X24" s="11"/>
@@ -3153,7 +3194,7 @@
       <c r="Z24" s="11"/>
       <c r="AA24" s="11"/>
     </row>
-    <row r="25" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
       <c r="X25" s="11"/>
@@ -3161,7 +3202,7 @@
       <c r="Z25" s="11"/>
       <c r="AA25" s="11"/>
     </row>
-    <row r="26" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="26" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V26" s="11"/>
       <c r="W26" s="11"/>
       <c r="X26" s="11"/>
@@ -3169,7 +3210,7 @@
       <c r="Z26" s="11"/>
       <c r="AA26" s="11"/>
     </row>
-    <row r="27" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
       <c r="X27" s="11"/>
@@ -3177,7 +3218,7 @@
       <c r="Z27" s="11"/>
       <c r="AA27" s="11"/>
     </row>
-    <row r="28" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
       <c r="X28" s="11"/>
@@ -3193,7 +3234,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3203,9 +3244,9 @@
       <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.35">
       <c r="B2" s="29" t="s">
         <v>24</v>
       </c>
@@ -3229,7 +3270,7 @@
       <c r="T2" s="29"/>
       <c r="U2" s="29"/>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.35">
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -3252,114 +3293,114 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.35">
       <c r="AH4" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
     </row>
-    <row r="6" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
     </row>
-    <row r="7" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
     </row>
-    <row r="8" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="11"/>
       <c r="Y8" s="11"/>
     </row>
-    <row r="9" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="11"/>
     </row>
-    <row r="10" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
     </row>
-    <row r="11" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
     </row>
-    <row r="12" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
       <c r="Y12" s="11"/>
     </row>
-    <row r="13" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="11"/>
     </row>
-    <row r="14" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
     </row>
-    <row r="15" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
     </row>
-    <row r="16" spans="2:34" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.35">
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
     </row>
-    <row r="17" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
     </row>
-    <row r="18" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
       <c r="Y18" s="11"/>
     </row>
-    <row r="19" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
       <c r="Y19" s="11"/>
     </row>
-    <row r="20" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
     </row>
-    <row r="21" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="22:27" x14ac:dyDescent="0.35">
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
     </row>
-    <row r="28" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="28" spans="22:27" x14ac:dyDescent="0.35">
       <c r="X28" s="12" t="s">
         <v>39</v>
       </c>
@@ -3371,7 +3412,7 @@
       </c>
       <c r="AA28" s="16"/>
     </row>
-    <row r="29" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="22:27" x14ac:dyDescent="0.35">
       <c r="X29" s="12" t="s">
         <v>40</v>
       </c>
@@ -3383,12 +3424,12 @@
       </c>
       <c r="AA29" s="16"/>
     </row>
-    <row r="32" spans="22:27" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="32" spans="22:27" x14ac:dyDescent="0.35">
       <c r="X32" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.35">
       <c r="Y33" t="s">
         <v>26</v>
       </c>
@@ -3399,7 +3440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.35">
       <c r="X34" t="s">
         <v>26</v>
       </c>
@@ -3414,7 +3455,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="35" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.35">
       <c r="X35" t="s">
         <v>27</v>
       </c>
@@ -3422,7 +3463,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.35">
       <c r="X36" t="s">
         <v>29</v>
       </c>
@@ -3430,13 +3471,13 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="37" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.35">
       <c r="Y37">
         <f>SUM(Y35:Y36)</f>
         <v>2150</v>
       </c>
     </row>
-    <row r="38" spans="2:28" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>28</v>
       </c>
@@ -3453,6 +3494,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3675,15 +3725,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3691,6 +3732,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8E92680-A115-41CF-8E05-8F9967A15F27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3709,14 +3758,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated med socio diskonteringsrate og HETCP
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
+++ b/TIMES-DE/SuppXLS/Trades/ScenTrade_TRADE_DE_ELC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C28E61-0999-4C52-8041-C8EA40BCBD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0CA5FD-FB11-478C-89B2-06F6717D9165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="68">
   <si>
     <t>Year</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Cset_CN</t>
   </si>
   <si>
-    <t>DKW</t>
-  </si>
-  <si>
     <t>ELCC</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>TU_ELCC_DE5_DE1_01</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -1656,8 +1656,8 @@
   </sheetPr>
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C15" s="9" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>10</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.35">
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="K40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.35">
@@ -2468,7 +2468,7 @@
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.35">
@@ -2552,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.35">
@@ -2633,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2679,25 +2679,23 @@
         <v>47</v>
       </c>
       <c r="I4" s="27"/>
-      <c r="J4" s="26" t="s">
-        <v>60</v>
-      </c>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="F5" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="G5" s="28">
         <v>2010</v>
@@ -2705,25 +2703,22 @@
       <c r="H5" s="28">
         <v>0.1</v>
       </c>
-      <c r="J5">
-        <v>0.10686678676759548</v>
-      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="28" t="s">
+      <c r="F6" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="G6" s="28">
         <v>2010</v>
@@ -2731,25 +2726,22 @@
       <c r="H6" s="28">
         <v>0.1</v>
       </c>
-      <c r="J6">
-        <v>2.4997560823677975E-2</v>
-      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="28" t="s">
+      <c r="F7" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="G7" s="28">
         <v>2010</v>
@@ -2757,34 +2749,28 @@
       <c r="H7" s="28">
         <v>0.1</v>
       </c>
-      <c r="J7">
-        <v>2.202997304070314E-2</v>
-      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="28" t="s">
+      <c r="F8" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="G8" s="28">
         <v>2010</v>
       </c>
       <c r="H8" s="28">
         <v>0.1</v>
-      </c>
-      <c r="J8">
-        <v>2.0027248218821018E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
@@ -2793,16 +2779,16 @@
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
         <v>61</v>
       </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>62</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
       </c>
       <c r="G9">
         <v>2050</v>
@@ -2817,16 +2803,16 @@
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>62</v>
-      </c>
-      <c r="F10" t="s">
-        <v>63</v>
       </c>
       <c r="G10">
         <v>2050</v>
@@ -2841,16 +2827,16 @@
         <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>63</v>
       </c>
       <c r="G11">
         <v>2050</v>
@@ -2865,16 +2851,16 @@
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
       </c>
       <c r="G12">
         <v>2050</v>
@@ -2889,16 +2875,16 @@
         <v>TU_ELCC_DE2_DE1_01</v>
       </c>
       <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2913,16 +2899,16 @@
         <v>TU_ELCC_DE3_DE1_01</v>
       </c>
       <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>63</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -2937,16 +2923,16 @@
         <v>TU_ELCC_DE4_DE1_01</v>
       </c>
       <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>63</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2961,16 +2947,16 @@
         <v>TU_ELCC_DE5_DE1_01</v>
       </c>
       <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>62</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3494,12 +3480,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3726,15 +3709,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3759,10 +3746,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B270BEA8-3E7E-48B6-A709-99E80E2955ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FCFB0AB-85DB-4F0E-94C0-B4D60677B4B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>